<commit_message>
Global comment and omnivox grades upload
</commit_message>
<xml_diff>
--- a/tests/fixtures/grille_gradebook.xlsx
+++ b/tests/fixtures/grille_gradebook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Git repo - prof/c3hm/tests/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Git repo - prof/c3hm/tests/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F35CCF-D58D-114D-B1A2-046527719D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FF7B2C-EA1C-4640-84CE-9D144DFC0CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,87 +18,90 @@
     <sheet name="gc_rhum" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="cthm_C2_comment" localSheetId="1">archibord!$J$14</definedName>
-    <definedName name="cthm_C2_comment" localSheetId="2">gc_rhum!$J$14</definedName>
-    <definedName name="cthm_C2_comment" localSheetId="0">houle!$J$14</definedName>
-    <definedName name="cthm_C2_grade" localSheetId="1">archibord!$I$14</definedName>
-    <definedName name="cthm_C2_grade" localSheetId="2">gc_rhum!$I$14</definedName>
-    <definedName name="cthm_C2_grade" localSheetId="0">houle!$I$14</definedName>
-    <definedName name="cthm_C2_I1_comment" localSheetId="1">archibord!$J$15</definedName>
-    <definedName name="cthm_C2_I1_comment" localSheetId="2">gc_rhum!$J$15</definedName>
-    <definedName name="cthm_C2_I1_comment" localSheetId="0">houle!$J$15</definedName>
-    <definedName name="cthm_C2_I1_grade" localSheetId="1">archibord!$G$15</definedName>
-    <definedName name="cthm_C2_I1_grade" localSheetId="2">gc_rhum!$G$15</definedName>
-    <definedName name="cthm_C2_I1_grade" localSheetId="0">houle!$G$15</definedName>
-    <definedName name="cthm_C2_I2_comment" localSheetId="1">archibord!$J$16</definedName>
-    <definedName name="cthm_C2_I2_comment" localSheetId="2">gc_rhum!$J$16</definedName>
-    <definedName name="cthm_C2_I2_comment" localSheetId="0">houle!$J$16</definedName>
-    <definedName name="cthm_C2_I2_grade" localSheetId="1">archibord!$G$16</definedName>
-    <definedName name="cthm_C2_I2_grade" localSheetId="2">gc_rhum!$G$16</definedName>
-    <definedName name="cthm_C2_I2_grade" localSheetId="0">houle!$G$16</definedName>
-    <definedName name="cthm_C2_I3_comment" localSheetId="1">archibord!$J$17</definedName>
-    <definedName name="cthm_C2_I3_comment" localSheetId="2">gc_rhum!$J$17</definedName>
-    <definedName name="cthm_C2_I3_comment" localSheetId="0">houle!$J$17</definedName>
-    <definedName name="cthm_C2_I3_grade" localSheetId="1">archibord!$G$17</definedName>
-    <definedName name="cthm_C2_I3_grade" localSheetId="2">gc_rhum!$G$17</definedName>
-    <definedName name="cthm_C2_I3_grade" localSheetId="0">houle!$G$17</definedName>
-    <definedName name="cthm_C3_comment" localSheetId="1">archibord!$J$18</definedName>
-    <definedName name="cthm_C3_comment" localSheetId="2">gc_rhum!$J$18</definedName>
-    <definedName name="cthm_C3_comment" localSheetId="0">houle!$J$18</definedName>
-    <definedName name="cthm_C3_grade" localSheetId="1">archibord!$I$18</definedName>
-    <definedName name="cthm_C3_grade" localSheetId="2">gc_rhum!$I$18</definedName>
-    <definedName name="cthm_C3_grade" localSheetId="0">houle!$I$18</definedName>
-    <definedName name="cthm_C3_I1_comment" localSheetId="1">archibord!$J$19</definedName>
-    <definedName name="cthm_C3_I1_comment" localSheetId="2">gc_rhum!$J$19</definedName>
-    <definedName name="cthm_C3_I1_comment" localSheetId="0">houle!$J$19</definedName>
-    <definedName name="cthm_C3_I1_grade" localSheetId="1">archibord!$G$19</definedName>
-    <definedName name="cthm_C3_I1_grade" localSheetId="2">gc_rhum!$G$19</definedName>
-    <definedName name="cthm_C3_I1_grade" localSheetId="0">houle!$G$19</definedName>
-    <definedName name="cthm_C3_I2_comment" localSheetId="1">archibord!$J$20</definedName>
-    <definedName name="cthm_C3_I2_comment" localSheetId="2">gc_rhum!$J$20</definedName>
-    <definedName name="cthm_C3_I2_comment" localSheetId="0">houle!$J$20</definedName>
-    <definedName name="cthm_C3_I2_grade" localSheetId="1">archibord!$G$20</definedName>
-    <definedName name="cthm_C3_I2_grade" localSheetId="2">gc_rhum!$G$20</definedName>
-    <definedName name="cthm_C3_I2_grade" localSheetId="0">houle!$G$20</definedName>
-    <definedName name="cthm_C3_I3_comment" localSheetId="1">archibord!$J$21</definedName>
-    <definedName name="cthm_C3_I3_comment" localSheetId="2">gc_rhum!$J$21</definedName>
-    <definedName name="cthm_C3_I3_comment" localSheetId="0">houle!$J$21</definedName>
-    <definedName name="cthm_C3_I3_grade" localSheetId="1">archibord!$G$21</definedName>
-    <definedName name="cthm_C3_I3_grade" localSheetId="2">gc_rhum!$G$21</definedName>
-    <definedName name="cthm_C3_I3_grade" localSheetId="0">houle!$G$21</definedName>
+    <definedName name="cthm_C2_comment" localSheetId="1">archibord!$J$15</definedName>
+    <definedName name="cthm_C2_comment" localSheetId="2">gc_rhum!$J$15</definedName>
+    <definedName name="cthm_C2_comment" localSheetId="0">houle!$J$15</definedName>
+    <definedName name="cthm_C2_grade" localSheetId="1">archibord!$I$15</definedName>
+    <definedName name="cthm_C2_grade" localSheetId="2">gc_rhum!$I$15</definedName>
+    <definedName name="cthm_C2_grade" localSheetId="0">houle!$I$15</definedName>
+    <definedName name="cthm_C2_I1_comment" localSheetId="1">archibord!$J$16</definedName>
+    <definedName name="cthm_C2_I1_comment" localSheetId="2">gc_rhum!$J$16</definedName>
+    <definedName name="cthm_C2_I1_comment" localSheetId="0">houle!$J$16</definedName>
+    <definedName name="cthm_C2_I1_grade" localSheetId="1">archibord!$G$16</definedName>
+    <definedName name="cthm_C2_I1_grade" localSheetId="2">gc_rhum!$G$16</definedName>
+    <definedName name="cthm_C2_I1_grade" localSheetId="0">houle!$G$16</definedName>
+    <definedName name="cthm_C2_I2_comment" localSheetId="1">archibord!$J$17</definedName>
+    <definedName name="cthm_C2_I2_comment" localSheetId="2">gc_rhum!$J$17</definedName>
+    <definedName name="cthm_C2_I2_comment" localSheetId="0">houle!$J$17</definedName>
+    <definedName name="cthm_C2_I2_grade" localSheetId="1">archibord!$G$17</definedName>
+    <definedName name="cthm_C2_I2_grade" localSheetId="2">gc_rhum!$G$17</definedName>
+    <definedName name="cthm_C2_I2_grade" localSheetId="0">houle!$G$17</definedName>
+    <definedName name="cthm_C2_I3_comment" localSheetId="1">archibord!$J$18</definedName>
+    <definedName name="cthm_C2_I3_comment" localSheetId="2">gc_rhum!$J$18</definedName>
+    <definedName name="cthm_C2_I3_comment" localSheetId="0">houle!$J$18</definedName>
+    <definedName name="cthm_C2_I3_grade" localSheetId="1">archibord!$G$18</definedName>
+    <definedName name="cthm_C2_I3_grade" localSheetId="2">gc_rhum!$G$18</definedName>
+    <definedName name="cthm_C2_I3_grade" localSheetId="0">houle!$G$18</definedName>
+    <definedName name="cthm_C3_comment" localSheetId="1">archibord!$J$19</definedName>
+    <definedName name="cthm_C3_comment" localSheetId="2">gc_rhum!$J$19</definedName>
+    <definedName name="cthm_C3_comment" localSheetId="0">houle!$J$19</definedName>
+    <definedName name="cthm_C3_grade" localSheetId="1">archibord!$I$19</definedName>
+    <definedName name="cthm_C3_grade" localSheetId="2">gc_rhum!$I$19</definedName>
+    <definedName name="cthm_C3_grade" localSheetId="0">houle!$I$19</definedName>
+    <definedName name="cthm_C3_I1_comment" localSheetId="1">archibord!$J$20</definedName>
+    <definedName name="cthm_C3_I1_comment" localSheetId="2">gc_rhum!$J$20</definedName>
+    <definedName name="cthm_C3_I1_comment" localSheetId="0">houle!$J$20</definedName>
+    <definedName name="cthm_C3_I1_grade" localSheetId="1">archibord!$G$20</definedName>
+    <definedName name="cthm_C3_I1_grade" localSheetId="2">gc_rhum!$G$20</definedName>
+    <definedName name="cthm_C3_I1_grade" localSheetId="0">houle!$G$20</definedName>
+    <definedName name="cthm_C3_I2_comment" localSheetId="1">archibord!$J$21</definedName>
+    <definedName name="cthm_C3_I2_comment" localSheetId="2">gc_rhum!$J$21</definedName>
+    <definedName name="cthm_C3_I2_comment" localSheetId="0">houle!$J$21</definedName>
+    <definedName name="cthm_C3_I2_grade" localSheetId="1">archibord!$G$21</definedName>
+    <definedName name="cthm_C3_I2_grade" localSheetId="2">gc_rhum!$G$21</definedName>
+    <definedName name="cthm_C3_I2_grade" localSheetId="0">houle!$G$21</definedName>
+    <definedName name="cthm_C3_I3_comment" localSheetId="1">archibord!$J$22</definedName>
+    <definedName name="cthm_C3_I3_comment" localSheetId="2">gc_rhum!$J$22</definedName>
+    <definedName name="cthm_C3_I3_comment" localSheetId="0">houle!$J$22</definedName>
+    <definedName name="cthm_C3_I3_grade" localSheetId="1">archibord!$G$22</definedName>
+    <definedName name="cthm_C3_I3_grade" localSheetId="2">gc_rhum!$G$22</definedName>
+    <definedName name="cthm_C3_I3_grade" localSheetId="0">houle!$G$22</definedName>
+    <definedName name="cthm_global_comment" localSheetId="1">archibord!$B$5</definedName>
+    <definedName name="cthm_global_comment" localSheetId="2">gc_rhum!$B$5</definedName>
+    <definedName name="cthm_global_comment" localSheetId="0">houle!$B$5</definedName>
     <definedName name="cthm_omnivox" localSheetId="1">archibord!$B$4</definedName>
     <definedName name="cthm_omnivox" localSheetId="2">gc_rhum!$B$4</definedName>
     <definedName name="cthm_omnivox" localSheetId="0">houle!$B$4</definedName>
-    <definedName name="lessivage_balai_comment" localSheetId="1">archibord!$J$10</definedName>
-    <definedName name="lessivage_balai_comment" localSheetId="2">gc_rhum!$J$10</definedName>
-    <definedName name="lessivage_balai_comment" localSheetId="0">houle!$J$10</definedName>
-    <definedName name="lessivage_balai_grade" localSheetId="1">archibord!$G$10</definedName>
-    <definedName name="lessivage_balai_grade" localSheetId="2">gc_rhum!$G$10</definedName>
-    <definedName name="lessivage_balai_grade" localSheetId="0">houle!$G$10</definedName>
-    <definedName name="lessivage_comment" localSheetId="1">archibord!$J$9</definedName>
-    <definedName name="lessivage_comment" localSheetId="2">gc_rhum!$J$9</definedName>
-    <definedName name="lessivage_comment" localSheetId="0">houle!$J$9</definedName>
-    <definedName name="lessivage_grade" localSheetId="1">archibord!$I$9</definedName>
-    <definedName name="lessivage_grade" localSheetId="2">gc_rhum!$I$9</definedName>
-    <definedName name="lessivage_grade" localSheetId="0">houle!$I$9</definedName>
-    <definedName name="lessivage_I2_comment" localSheetId="1">archibord!$J$11</definedName>
-    <definedName name="lessivage_I2_comment" localSheetId="2">gc_rhum!$J$11</definedName>
-    <definedName name="lessivage_I2_comment" localSheetId="0">houle!$J$11</definedName>
-    <definedName name="lessivage_I2_grade" localSheetId="1">archibord!$G$11</definedName>
-    <definedName name="lessivage_I2_grade" localSheetId="2">gc_rhum!$G$11</definedName>
-    <definedName name="lessivage_I2_grade" localSheetId="0">houle!$G$11</definedName>
-    <definedName name="lessivage_I3_comment" localSheetId="1">archibord!$J$12</definedName>
-    <definedName name="lessivage_I3_comment" localSheetId="2">gc_rhum!$J$12</definedName>
-    <definedName name="lessivage_I3_comment" localSheetId="0">houle!$J$12</definedName>
-    <definedName name="lessivage_I3_grade" localSheetId="1">archibord!$G$12</definedName>
-    <definedName name="lessivage_I3_grade" localSheetId="2">gc_rhum!$G$12</definedName>
-    <definedName name="lessivage_I3_grade" localSheetId="0">houle!$G$12</definedName>
-    <definedName name="lessivage_I4_comment" localSheetId="1">archibord!$J$13</definedName>
-    <definedName name="lessivage_I4_comment" localSheetId="2">gc_rhum!$J$13</definedName>
-    <definedName name="lessivage_I4_comment" localSheetId="0">houle!$J$13</definedName>
-    <definedName name="lessivage_I4_grade" localSheetId="1">archibord!$G$13</definedName>
-    <definedName name="lessivage_I4_grade" localSheetId="2">gc_rhum!$G$13</definedName>
-    <definedName name="lessivage_I4_grade" localSheetId="0">houle!$G$13</definedName>
+    <definedName name="lessivage_balai_comment" localSheetId="1">archibord!$J$11</definedName>
+    <definedName name="lessivage_balai_comment" localSheetId="2">gc_rhum!$J$11</definedName>
+    <definedName name="lessivage_balai_comment" localSheetId="0">houle!$J$11</definedName>
+    <definedName name="lessivage_balai_grade" localSheetId="1">archibord!$G$11</definedName>
+    <definedName name="lessivage_balai_grade" localSheetId="2">gc_rhum!$G$11</definedName>
+    <definedName name="lessivage_balai_grade" localSheetId="0">houle!$G$11</definedName>
+    <definedName name="lessivage_comment" localSheetId="1">archibord!$J$10</definedName>
+    <definedName name="lessivage_comment" localSheetId="2">gc_rhum!$J$10</definedName>
+    <definedName name="lessivage_comment" localSheetId="0">houle!$J$10</definedName>
+    <definedName name="lessivage_grade" localSheetId="1">archibord!$I$10</definedName>
+    <definedName name="lessivage_grade" localSheetId="2">gc_rhum!$I$10</definedName>
+    <definedName name="lessivage_grade" localSheetId="0">houle!$I$10</definedName>
+    <definedName name="lessivage_I2_comment" localSheetId="1">archibord!$J$12</definedName>
+    <definedName name="lessivage_I2_comment" localSheetId="2">gc_rhum!$J$12</definedName>
+    <definedName name="lessivage_I2_comment" localSheetId="0">houle!$J$12</definedName>
+    <definedName name="lessivage_I2_grade" localSheetId="1">archibord!$G$12</definedName>
+    <definedName name="lessivage_I2_grade" localSheetId="2">gc_rhum!$G$12</definedName>
+    <definedName name="lessivage_I2_grade" localSheetId="0">houle!$G$12</definedName>
+    <definedName name="lessivage_I3_comment" localSheetId="1">archibord!$J$13</definedName>
+    <definedName name="lessivage_I3_comment" localSheetId="2">gc_rhum!$J$13</definedName>
+    <definedName name="lessivage_I3_comment" localSheetId="0">houle!$J$13</definedName>
+    <definedName name="lessivage_I3_grade" localSheetId="1">archibord!$G$13</definedName>
+    <definedName name="lessivage_I3_grade" localSheetId="2">gc_rhum!$G$13</definedName>
+    <definedName name="lessivage_I3_grade" localSheetId="0">houle!$G$13</definedName>
+    <definedName name="lessivage_I4_comment" localSheetId="1">archibord!$J$14</definedName>
+    <definedName name="lessivage_I4_comment" localSheetId="2">gc_rhum!$J$14</definedName>
+    <definedName name="lessivage_I4_comment" localSheetId="0">houle!$J$14</definedName>
+    <definedName name="lessivage_I4_grade" localSheetId="1">archibord!$G$14</definedName>
+    <definedName name="lessivage_I4_grade" localSheetId="2">gc_rhum!$G$14</definedName>
+    <definedName name="lessivage_I4_grade" localSheetId="0">houle!$G$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -118,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="51">
   <si>
     <t>Grille d'évaluation – 420-C3HM-MA – Le Grand Carénage des Flibustiers</t>
   </si>
@@ -135,6 +138,9 @@
     <t>314159</t>
   </si>
   <si>
+    <t>Commentaire général</t>
+  </si>
+  <si>
     <t>Total sur 50 pts</t>
   </si>
   <si>
@@ -171,40 +177,40 @@
     <t>Grand lessivage du pont</t>
   </si>
   <si>
-    <t>Balai brandi comme un sabre en pleine mêlée.</t>
-  </si>
-  <si>
-    <t>Seau d’eau salée renversé avec panache.</t>
-  </si>
-  <si>
-    <t>Mousse digne d’un kraken en plein spasme.</t>
-  </si>
-  <si>
-    <t>Chant marin entonné en chœur pour stimuler l’équipage.</t>
+    <t>Balai brandi comme un sabre en pleine mêlée</t>
+  </si>
+  <si>
+    <t>Seau d’eau salée renversé avec panache</t>
+  </si>
+  <si>
+    <t>Mousse digne d’un kraken en plein spasme</t>
+  </si>
+  <si>
+    <t>Chant marin entonné en chœur pour stimuler l’équipage</t>
   </si>
   <si>
     <t>Hissage du pavillon noir</t>
   </si>
   <si>
-    <t>Cordage enroulé en huit impeccable.</t>
-  </si>
-  <si>
-    <t>Pavillon solidement fixé au mât.</t>
-  </si>
-  <si>
-    <t>Drisse tendue sans nœud lâche.</t>
+    <t>Cordage enroulé en huit impeccable</t>
+  </si>
+  <si>
+    <t>Pavillon solidement fixé au mât</t>
+  </si>
+  <si>
+    <t>Drisse tendue sans nœud lâche</t>
   </si>
   <si>
     <t>Distribution du rhum</t>
   </si>
   <si>
-    <t>Gobelets remplis jusqu’à ras bord.</t>
-  </si>
-  <si>
-    <t>File d’attente de matelots respectée.</t>
-  </si>
-  <si>
-    <t>Toast improvisé incluant le capitaine.</t>
+    <t>Gobelets remplis jusqu’à ras bord</t>
+  </si>
+  <si>
+    <t>File d’attente de matelots respectée</t>
+  </si>
+  <si>
+    <t>Toast improvisé incluant le capitaine</t>
   </si>
   <si>
     <t>Moussaillon ArchiBord</t>
@@ -259,6 +265,15 @@
   </si>
   <si>
     <t>Commentaire 13</t>
+  </si>
+  <si>
+    <t>Excellent travail !</t>
+  </si>
+  <si>
+    <t>Aye Aye Aye</t>
+  </si>
+  <si>
+    <t>Tu es sur la bonne voie</t>
   </si>
 </sst>
 </file>
@@ -268,7 +283,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,12 +342,6 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -481,7 +490,31 @@
     <cellStyle name="Titre 3" xfId="5" builtinId="18"/>
     <cellStyle name="Titre 4" xfId="4" builtinId="19"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="48">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF0FFB0"/>
+          <bgColor rgb="FFF0FFB0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF0FFB0"/>
+          <bgColor rgb="FFF0FFB0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF0FFB0"/>
+          <bgColor rgb="FFF0FFB0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1140,10 +1173,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1175,108 +1208,85 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
-        <f>SUM(I9,I14,I18)</f>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <f>SUM(I10,I15,I19)</f>
         <v>46.270833333333336</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="5" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="F9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="H9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="I9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="J9" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="K9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="3">
-        <f>SUM(G10:G13)/SUM(K10:K13) * K9</f>
+    </row>
+    <row r="10" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="3">
+        <f>SUM(G11:G14)/SUM(K11:K14) * K10</f>
         <v>14.4375</v>
       </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="3">
-        <f>IF(ISBLANK(H9),G9,H9)</f>
+      <c r="H10" s="11"/>
+      <c r="I10" s="3">
+        <f>IF(ISBLANK(H10),G10,H10)</f>
         <v>14.4375</v>
-      </c>
-      <c r="J9" t="s">
-        <v>34</v>
-      </c>
-      <c r="K9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="13">
-        <f>IF(IF(ISBLANK(B10),0,1) + IF(ISBLANK(C10),0,1) + IF(ISBLANK(D10),0,1) + IF(ISBLANK(E10),0,1) + IF(ISBLANK(F10),0,1) = 1,IF(IF(ISBLANK(B10),0,IF(ISNUMBER(B10),B10,K10)) + IF(ISBLANK(C10),0,IF(ISNUMBER(C10),C10,L10)) + IF(ISBLANK(D10),0,IF(ISNUMBER(D10),D10,M10)) + IF(ISBLANK(E10),0,IF(ISNUMBER(E10),E10,N10)) + IF(ISBLANK(F10),0,IF(ISNUMBER(F10),F10,O10)) &gt; K10, NA(), IF(ISBLANK(B10),0,IF(ISNUMBER(B10),B10,K10)) + IF(ISBLANK(C10),0,IF(ISNUMBER(C10),C10,L10)) + IF(ISBLANK(D10),0,IF(ISNUMBER(D10),D10,M10)) + IF(ISBLANK(E10),0,IF(ISNUMBER(E10),E10,N10)) + IF(ISBLANK(F10),0,IF(ISNUMBER(F10),F10,O10))),NA())</f>
-        <v>20</v>
       </c>
       <c r="J10" t="s">
         <v>35</v>
       </c>
-      <c r="K10" s="12">
-        <v>20</v>
-      </c>
-      <c r="L10" s="12">
-        <v>17</v>
-      </c>
-      <c r="M10" s="12">
+      <c r="K10">
         <v>15</v>
-      </c>
-      <c r="N10" s="12">
-        <v>13</v>
-      </c>
-      <c r="O10" s="12">
-        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" t="s">
-        <v>33</v>
+      <c r="B11" s="12" t="s">
+        <v>34</v>
       </c>
       <c r="G11" s="13">
         <f>IF(IF(ISBLANK(B11),0,1) + IF(ISBLANK(C11),0,1) + IF(ISBLANK(D11),0,1) + IF(ISBLANK(E11),0,1) + IF(ISBLANK(F11),0,1) = 1,IF(IF(ISBLANK(B11),0,IF(ISNUMBER(B11),B11,K11)) + IF(ISBLANK(C11),0,IF(ISNUMBER(C11),C11,L11)) + IF(ISBLANK(D11),0,IF(ISNUMBER(D11),D11,M11)) + IF(ISBLANK(E11),0,IF(ISNUMBER(E11),E11,N11)) + IF(ISBLANK(F11),0,IF(ISNUMBER(F11),F11,O11)) &gt; K11, NA(), IF(ISBLANK(B11),0,IF(ISNUMBER(B11),B11,K11)) + IF(ISBLANK(C11),0,IF(ISNUMBER(C11),C11,L11)) + IF(ISBLANK(D11),0,IF(ISNUMBER(D11),D11,M11)) + IF(ISBLANK(E11),0,IF(ISNUMBER(E11),E11,N11)) + IF(ISBLANK(F11),0,IF(ISNUMBER(F11),F11,O11))),NA())</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J11" t="s">
         <v>36</v>
@@ -1301,12 +1311,13 @@
       <c r="A12" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>33</v>
+      <c r="B12" s="12"/>
+      <c r="C12" t="s">
+        <v>34</v>
       </c>
       <c r="G12" s="13">
         <f>IF(IF(ISBLANK(B12),0,1) + IF(ISBLANK(C12),0,1) + IF(ISBLANK(D12),0,1) + IF(ISBLANK(E12),0,1) + IF(ISBLANK(F12),0,1) = 1,IF(IF(ISBLANK(B12),0,IF(ISNUMBER(B12),B12,K12)) + IF(ISBLANK(C12),0,IF(ISNUMBER(C12),C12,L12)) + IF(ISBLANK(D12),0,IF(ISNUMBER(D12),D12,M12)) + IF(ISBLANK(E12),0,IF(ISNUMBER(E12),E12,N12)) + IF(ISBLANK(F12),0,IF(ISNUMBER(F12),F12,O12)) &gt; K12, NA(), IF(ISBLANK(B12),0,IF(ISNUMBER(B12),B12,K12)) + IF(ISBLANK(C12),0,IF(ISNUMBER(C12),C12,L12)) + IF(ISBLANK(D12),0,IF(ISNUMBER(D12),D12,M12)) + IF(ISBLANK(E12),0,IF(ISNUMBER(E12),E12,N12)) + IF(ISBLANK(F12),0,IF(ISNUMBER(F12),F12,O12))),NA())</f>
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J12" t="s">
         <v>37</v>
@@ -1332,7 +1343,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G13" s="13">
         <f>IF(IF(ISBLANK(B13),0,1) + IF(ISBLANK(C13),0,1) + IF(ISBLANK(D13),0,1) + IF(ISBLANK(E13),0,1) + IF(ISBLANK(F13),0,1) = 1,IF(IF(ISBLANK(B13),0,IF(ISNUMBER(B13),B13,K13)) + IF(ISBLANK(C13),0,IF(ISNUMBER(C13),C13,L13)) + IF(ISBLANK(D13),0,IF(ISNUMBER(D13),D13,M13)) + IF(ISBLANK(E13),0,IF(ISNUMBER(E13),E13,N13)) + IF(ISBLANK(F13),0,IF(ISNUMBER(F13),F13,O13)) &gt; K13, NA(), IF(ISBLANK(B13),0,IF(ISNUMBER(B13),B13,K13)) + IF(ISBLANK(C13),0,IF(ISNUMBER(C13),C13,L13)) + IF(ISBLANK(D13),0,IF(ISNUMBER(D13),D13,M13)) + IF(ISBLANK(E13),0,IF(ISNUMBER(E13),E13,N13)) + IF(ISBLANK(F13),0,IF(ISNUMBER(F13),F13,O13))),NA())</f>
@@ -1358,66 +1369,65 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="3">
-        <f>SUM(G15:G17)/SUM(K15:K17) * K14</f>
-        <v>17.333333333333336</v>
-      </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="3">
-        <f>IF(ISBLANK(H14),G14,H14)</f>
-        <v>17.333333333333336</v>
+      <c r="B14" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="13">
+        <f>IF(IF(ISBLANK(B14),0,1) + IF(ISBLANK(C14),0,1) + IF(ISBLANK(D14),0,1) + IF(ISBLANK(E14),0,1) + IF(ISBLANK(F14),0,1) = 1,IF(IF(ISBLANK(B14),0,IF(ISNUMBER(B14),B14,K14)) + IF(ISBLANK(C14),0,IF(ISNUMBER(C14),C14,L14)) + IF(ISBLANK(D14),0,IF(ISNUMBER(D14),D14,M14)) + IF(ISBLANK(E14),0,IF(ISNUMBER(E14),E14,N14)) + IF(ISBLANK(F14),0,IF(ISNUMBER(F14),F14,O14)) &gt; K14, NA(), IF(ISBLANK(B14),0,IF(ISNUMBER(B14),B14,K14)) + IF(ISBLANK(C14),0,IF(ISNUMBER(C14),C14,L14)) + IF(ISBLANK(D14),0,IF(ISNUMBER(D14),D14,M14)) + IF(ISBLANK(E14),0,IF(ISNUMBER(E14),E14,N14)) + IF(ISBLANK(F14),0,IF(ISNUMBER(F14),F14,O14))),NA())</f>
+        <v>20</v>
       </c>
       <c r="J14" t="s">
         <v>39</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="12">
         <v>20</v>
       </c>
+      <c r="L14" s="12">
+        <v>17</v>
+      </c>
+      <c r="M14" s="12">
+        <v>15</v>
+      </c>
+      <c r="N14" s="12">
+        <v>13</v>
+      </c>
+      <c r="O14" s="12">
+        <v>11</v>
+      </c>
     </row>
     <row r="15" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="13">
-        <f>IF(IF(ISBLANK(B15),0,1) + IF(ISBLANK(C15),0,1) + IF(ISBLANK(D15),0,1) + IF(ISBLANK(E15),0,1) + IF(ISBLANK(F15),0,1) = 1,IF(IF(ISBLANK(B15),0,IF(ISNUMBER(B15),B15,K15)) + IF(ISBLANK(C15),0,IF(ISNUMBER(C15),C15,L15)) + IF(ISBLANK(D15),0,IF(ISNUMBER(D15),D15,M15)) + IF(ISBLANK(E15),0,IF(ISNUMBER(E15),E15,N15)) + IF(ISBLANK(F15),0,IF(ISNUMBER(F15),F15,O15)) &gt; K15, NA(), IF(ISBLANK(B15),0,IF(ISNUMBER(B15),B15,K15)) + IF(ISBLANK(C15),0,IF(ISNUMBER(C15),C15,L15)) + IF(ISBLANK(D15),0,IF(ISNUMBER(D15),D15,M15)) + IF(ISBLANK(E15),0,IF(ISNUMBER(E15),E15,N15)) + IF(ISBLANK(F15),0,IF(ISNUMBER(F15),F15,O15))),NA())</f>
-        <v>5</v>
+      <c r="G15" s="3">
+        <f>SUM(G16:G18)/SUM(K16:K18) * K15</f>
+        <v>17.333333333333336</v>
+      </c>
+      <c r="H15" s="11"/>
+      <c r="I15" s="3">
+        <f>IF(ISBLANK(H15),G15,H15)</f>
+        <v>17.333333333333336</v>
       </c>
       <c r="J15" t="s">
         <v>40</v>
       </c>
-      <c r="K15" s="12">
-        <v>5</v>
-      </c>
-      <c r="L15" s="12">
-        <v>4</v>
-      </c>
-      <c r="M15" s="12">
-        <v>3</v>
-      </c>
-      <c r="N15" s="12">
-        <v>2</v>
-      </c>
-      <c r="O15" s="12">
-        <v>0</v>
+      <c r="K15">
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" t="s">
-        <v>33</v>
+      <c r="B16" s="12" t="s">
+        <v>34</v>
       </c>
       <c r="G16" s="13">
         <f>IF(IF(ISBLANK(B16),0,1) + IF(ISBLANK(C16),0,1) + IF(ISBLANK(D16),0,1) + IF(ISBLANK(E16),0,1) + IF(ISBLANK(F16),0,1) = 1,IF(IF(ISBLANK(B16),0,IF(ISNUMBER(B16),B16,K16)) + IF(ISBLANK(C16),0,IF(ISNUMBER(C16),C16,L16)) + IF(ISBLANK(D16),0,IF(ISNUMBER(D16),D16,M16)) + IF(ISBLANK(E16),0,IF(ISNUMBER(E16),E16,N16)) + IF(ISBLANK(F16),0,IF(ISNUMBER(F16),F16,O16)) &gt; K16, NA(), IF(ISBLANK(B16),0,IF(ISNUMBER(B16),B16,K16)) + IF(ISBLANK(C16),0,IF(ISNUMBER(C16),C16,L16)) + IF(ISBLANK(D16),0,IF(ISNUMBER(D16),D16,M16)) + IF(ISBLANK(E16),0,IF(ISNUMBER(E16),E16,N16)) + IF(ISBLANK(F16),0,IF(ISNUMBER(F16),F16,O16))),NA())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J16" t="s">
         <v>41</v>
@@ -1444,7 +1454,7 @@
       </c>
       <c r="B17" s="12"/>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G17" s="13">
         <f>IF(IF(ISBLANK(B17),0,1) + IF(ISBLANK(C17),0,1) + IF(ISBLANK(D17),0,1) + IF(ISBLANK(E17),0,1) + IF(ISBLANK(F17),0,1) = 1,IF(IF(ISBLANK(B17),0,IF(ISNUMBER(B17),B17,K17)) + IF(ISBLANK(C17),0,IF(ISNUMBER(C17),C17,L17)) + IF(ISBLANK(D17),0,IF(ISNUMBER(D17),D17,M17)) + IF(ISBLANK(E17),0,IF(ISNUMBER(E17),E17,N17)) + IF(ISBLANK(F17),0,IF(ISNUMBER(F17),F17,O17)) &gt; K17, NA(), IF(ISBLANK(B17),0,IF(ISNUMBER(B17),B17,K17)) + IF(ISBLANK(C17),0,IF(ISNUMBER(C17),C17,L17)) + IF(ISBLANK(D17),0,IF(ISNUMBER(D17),D17,M17)) + IF(ISBLANK(E17),0,IF(ISNUMBER(E17),E17,N17)) + IF(ISBLANK(F17),0,IF(ISNUMBER(F17),F17,O17))),NA())</f>
@@ -1470,66 +1480,67 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="3">
-        <f>SUM(G19:G21)/SUM(K19:K21) * K18</f>
-        <v>14.5</v>
-      </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="3">
-        <f>IF(ISBLANK(H18),G18,H18)</f>
-        <v>14.5</v>
+      <c r="B18" s="12"/>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="13">
+        <f>IF(IF(ISBLANK(B18),0,1) + IF(ISBLANK(C18),0,1) + IF(ISBLANK(D18),0,1) + IF(ISBLANK(E18),0,1) + IF(ISBLANK(F18),0,1) = 1,IF(IF(ISBLANK(B18),0,IF(ISNUMBER(B18),B18,K18)) + IF(ISBLANK(C18),0,IF(ISNUMBER(C18),C18,L18)) + IF(ISBLANK(D18),0,IF(ISNUMBER(D18),D18,M18)) + IF(ISBLANK(E18),0,IF(ISNUMBER(E18),E18,N18)) + IF(ISBLANK(F18),0,IF(ISNUMBER(F18),F18,O18)) &gt; K18, NA(), IF(ISBLANK(B18),0,IF(ISNUMBER(B18),B18,K18)) + IF(ISBLANK(C18),0,IF(ISNUMBER(C18),C18,L18)) + IF(ISBLANK(D18),0,IF(ISNUMBER(D18),D18,M18)) + IF(ISBLANK(E18),0,IF(ISNUMBER(E18),E18,N18)) + IF(ISBLANK(F18),0,IF(ISNUMBER(F18),F18,O18))),NA())</f>
+        <v>4</v>
       </c>
       <c r="J18" t="s">
         <v>43</v>
       </c>
-      <c r="K18">
-        <v>15</v>
+      <c r="K18" s="12">
+        <v>5</v>
+      </c>
+      <c r="L18" s="12">
+        <v>4</v>
+      </c>
+      <c r="M18" s="12">
+        <v>3</v>
+      </c>
+      <c r="N18" s="12">
+        <v>2</v>
+      </c>
+      <c r="O18" s="12">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="13">
-        <f>IF(IF(ISBLANK(B19),0,1) + IF(ISBLANK(C19),0,1) + IF(ISBLANK(D19),0,1) + IF(ISBLANK(E19),0,1) + IF(ISBLANK(F19),0,1) = 1,IF(IF(ISBLANK(B19),0,IF(ISNUMBER(B19),B19,K19)) + IF(ISBLANK(C19),0,IF(ISNUMBER(C19),C19,L19)) + IF(ISBLANK(D19),0,IF(ISNUMBER(D19),D19,M19)) + IF(ISBLANK(E19),0,IF(ISNUMBER(E19),E19,N19)) + IF(ISBLANK(F19),0,IF(ISNUMBER(F19),F19,O19)) &gt; K19, NA(), IF(ISBLANK(B19),0,IF(ISNUMBER(B19),B19,K19)) + IF(ISBLANK(C19),0,IF(ISNUMBER(C19),C19,L19)) + IF(ISBLANK(D19),0,IF(ISNUMBER(D19),D19,M19)) + IF(ISBLANK(E19),0,IF(ISNUMBER(E19),E19,N19)) + IF(ISBLANK(F19),0,IF(ISNUMBER(F19),F19,O19))),NA())</f>
-        <v>4</v>
+      <c r="G19" s="3">
+        <f>SUM(G20:G22)/SUM(K20:K22) * K19</f>
+        <v>14.5</v>
+      </c>
+      <c r="H19" s="11"/>
+      <c r="I19" s="3">
+        <f>IF(ISBLANK(H19),G19,H19)</f>
+        <v>14.5</v>
       </c>
       <c r="J19" t="s">
         <v>44</v>
       </c>
-      <c r="K19" s="12">
-        <v>5</v>
-      </c>
-      <c r="L19" s="12">
-        <v>4</v>
-      </c>
-      <c r="M19" s="12">
-        <v>3</v>
-      </c>
-      <c r="N19" s="12">
-        <v>2</v>
-      </c>
-      <c r="O19" s="12">
-        <v>0</v>
+      <c r="K19">
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>33</v>
+      <c r="B20" s="12"/>
+      <c r="C20" t="s">
+        <v>34</v>
       </c>
       <c r="G20" s="13">
         <f>IF(IF(ISBLANK(B20),0,1) + IF(ISBLANK(C20),0,1) + IF(ISBLANK(D20),0,1) + IF(ISBLANK(E20),0,1) + IF(ISBLANK(F20),0,1) = 1,IF(IF(ISBLANK(B20),0,IF(ISNUMBER(B20),B20,K20)) + IF(ISBLANK(C20),0,IF(ISNUMBER(C20),C20,L20)) + IF(ISBLANK(D20),0,IF(ISNUMBER(D20),D20,M20)) + IF(ISBLANK(E20),0,IF(ISNUMBER(E20),E20,N20)) + IF(ISBLANK(F20),0,IF(ISNUMBER(F20),F20,O20)) &gt; K20, NA(), IF(ISBLANK(B20),0,IF(ISNUMBER(B20),B20,K20)) + IF(ISBLANK(C20),0,IF(ISNUMBER(C20),C20,L20)) + IF(ISBLANK(D20),0,IF(ISNUMBER(D20),D20,M20)) + IF(ISBLANK(E20),0,IF(ISNUMBER(E20),E20,N20)) + IF(ISBLANK(F20),0,IF(ISNUMBER(F20),F20,O20))),NA())</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J20" t="s">
         <v>45</v>
@@ -1555,106 +1566,135 @@
         <v>28</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G21" s="13">
         <f>IF(IF(ISBLANK(B21),0,1) + IF(ISBLANK(C21),0,1) + IF(ISBLANK(D21),0,1) + IF(ISBLANK(E21),0,1) + IF(ISBLANK(F21),0,1) = 1,IF(IF(ISBLANK(B21),0,IF(ISNUMBER(B21),B21,K21)) + IF(ISBLANK(C21),0,IF(ISNUMBER(C21),C21,L21)) + IF(ISBLANK(D21),0,IF(ISNUMBER(D21),D21,M21)) + IF(ISBLANK(E21),0,IF(ISNUMBER(E21),E21,N21)) + IF(ISBLANK(F21),0,IF(ISNUMBER(F21),F21,O21)) &gt; K21, NA(), IF(ISBLANK(B21),0,IF(ISNUMBER(B21),B21,K21)) + IF(ISBLANK(C21),0,IF(ISNUMBER(C21),C21,L21)) + IF(ISBLANK(D21),0,IF(ISNUMBER(D21),D21,M21)) + IF(ISBLANK(E21),0,IF(ISNUMBER(E21),E21,N21)) + IF(ISBLANK(F21),0,IF(ISNUMBER(F21),F21,O21))),NA())</f>
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="J21" t="s">
         <v>46</v>
       </c>
       <c r="K21" s="12">
+        <v>5</v>
+      </c>
+      <c r="L21" s="12">
+        <v>4</v>
+      </c>
+      <c r="M21" s="12">
+        <v>3</v>
+      </c>
+      <c r="N21" s="12">
+        <v>2</v>
+      </c>
+      <c r="O21" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="13">
+        <f>IF(IF(ISBLANK(B22),0,1) + IF(ISBLANK(C22),0,1) + IF(ISBLANK(D22),0,1) + IF(ISBLANK(E22),0,1) + IF(ISBLANK(F22),0,1) = 1,IF(IF(ISBLANK(B22),0,IF(ISNUMBER(B22),B22,K22)) + IF(ISBLANK(C22),0,IF(ISNUMBER(C22),C22,L22)) + IF(ISBLANK(D22),0,IF(ISNUMBER(D22),D22,M22)) + IF(ISBLANK(E22),0,IF(ISNUMBER(E22),E22,N22)) + IF(ISBLANK(F22),0,IF(ISNUMBER(F22),F22,O22)) &gt; K22, NA(), IF(ISBLANK(B22),0,IF(ISNUMBER(B22),B22,K22)) + IF(ISBLANK(C22),0,IF(ISNUMBER(C22),C22,L22)) + IF(ISBLANK(D22),0,IF(ISNUMBER(D22),D22,M22)) + IF(ISBLANK(E22),0,IF(ISNUMBER(E22),E22,N22)) + IF(ISBLANK(F22),0,IF(ISNUMBER(F22),F22,O22))),NA())</f>
         <v>20</v>
       </c>
-      <c r="L21" s="12">
+      <c r="J22" t="s">
+        <v>47</v>
+      </c>
+      <c r="K22" s="12">
+        <v>20</v>
+      </c>
+      <c r="L22" s="12">
         <v>17</v>
       </c>
-      <c r="M21" s="12">
+      <c r="M22" s="12">
         <v>15</v>
       </c>
-      <c r="N21" s="12">
+      <c r="N22" s="12">
         <v>13</v>
       </c>
-      <c r="O21" s="12">
+      <c r="O22" s="12">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <conditionalFormatting sqref="B10:B13">
-    <cfRule type="expression" dxfId="44" priority="1" stopIfTrue="1">
-      <formula>NOT(ISBLANK(B10))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15:B17">
-    <cfRule type="expression" dxfId="43" priority="21" stopIfTrue="1">
-      <formula>NOT(ISBLANK(B15))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19:B21">
-    <cfRule type="expression" dxfId="42" priority="36" stopIfTrue="1">
-      <formula>NOT(ISBLANK(B19))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10:C13">
-    <cfRule type="expression" dxfId="41" priority="2" stopIfTrue="1">
-      <formula>NOT(ISBLANK(C10))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15:C17">
-    <cfRule type="expression" dxfId="40" priority="22" stopIfTrue="1">
-      <formula>NOT(ISBLANK(C15))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19:C21">
-    <cfRule type="expression" dxfId="39" priority="37" stopIfTrue="1">
-      <formula>NOT(ISBLANK(C19))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D10:D13">
-    <cfRule type="expression" dxfId="38" priority="3" stopIfTrue="1">
-      <formula>NOT(ISBLANK(D10))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D15:D17">
-    <cfRule type="expression" dxfId="37" priority="23" stopIfTrue="1">
-      <formula>NOT(ISBLANK(D15))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D19:D21">
-    <cfRule type="expression" dxfId="36" priority="38" stopIfTrue="1">
-      <formula>NOT(ISBLANK(D19))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E10:E13">
-    <cfRule type="expression" dxfId="35" priority="4" stopIfTrue="1">
-      <formula>NOT(ISBLANK(E10))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E15:E17">
-    <cfRule type="expression" dxfId="34" priority="24" stopIfTrue="1">
-      <formula>NOT(ISBLANK(E15))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E19:E21">
-    <cfRule type="expression" dxfId="33" priority="39" stopIfTrue="1">
-      <formula>NOT(ISBLANK(E19))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F10:F13">
-    <cfRule type="expression" dxfId="32" priority="5" stopIfTrue="1">
-      <formula>NOT(ISBLANK(F10))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F15:F17">
-    <cfRule type="expression" dxfId="31" priority="25" stopIfTrue="1">
-      <formula>NOT(ISBLANK(F15))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F19:F21">
-    <cfRule type="expression" dxfId="30" priority="40" stopIfTrue="1">
-      <formula>NOT(ISBLANK(F19))</formula>
+  <conditionalFormatting sqref="B11:B14">
+    <cfRule type="expression" dxfId="47" priority="1" stopIfTrue="1">
+      <formula>NOT(ISBLANK(B11))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16:B18">
+    <cfRule type="expression" dxfId="46" priority="21" stopIfTrue="1">
+      <formula>NOT(ISBLANK(B16))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20:B22">
+    <cfRule type="expression" dxfId="45" priority="36" stopIfTrue="1">
+      <formula>NOT(ISBLANK(B20))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:C14">
+    <cfRule type="expression" dxfId="44" priority="2" stopIfTrue="1">
+      <formula>NOT(ISBLANK(C11))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16:C18">
+    <cfRule type="expression" dxfId="43" priority="22" stopIfTrue="1">
+      <formula>NOT(ISBLANK(C16))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20:C22">
+    <cfRule type="expression" dxfId="42" priority="37" stopIfTrue="1">
+      <formula>NOT(ISBLANK(C20))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11:D14">
+    <cfRule type="expression" dxfId="41" priority="3" stopIfTrue="1">
+      <formula>NOT(ISBLANK(D11))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:D18">
+    <cfRule type="expression" dxfId="40" priority="23" stopIfTrue="1">
+      <formula>NOT(ISBLANK(D16))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20:D22">
+    <cfRule type="expression" dxfId="39" priority="38" stopIfTrue="1">
+      <formula>NOT(ISBLANK(D20))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11:E14">
+    <cfRule type="expression" dxfId="38" priority="4" stopIfTrue="1">
+      <formula>NOT(ISBLANK(E11))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16:E18">
+    <cfRule type="expression" dxfId="37" priority="24" stopIfTrue="1">
+      <formula>NOT(ISBLANK(E16))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20:E22">
+    <cfRule type="expression" dxfId="36" priority="39" stopIfTrue="1">
+      <formula>NOT(ISBLANK(E20))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11:F14">
+    <cfRule type="expression" dxfId="35" priority="5" stopIfTrue="1">
+      <formula>NOT(ISBLANK(F11))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16:F18">
+    <cfRule type="expression" dxfId="34" priority="25" stopIfTrue="1">
+      <formula>NOT(ISBLANK(F16))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20:F22">
+    <cfRule type="expression" dxfId="33" priority="40" stopIfTrue="1">
+      <formula>NOT(ISBLANK(F20))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1663,10 +1703,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1687,7 +1727,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -1695,96 +1735,76 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
-        <f>SUM(I9,I14,I18)</f>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <f>SUM(I10,I15,I19)</f>
         <v>27.625</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="5" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="F9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="H9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="I9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="J9" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="K9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="3">
-        <f>SUM(G10:G13)/SUM(K10:K13) * K9</f>
+    </row>
+    <row r="10" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="3">
+        <f>SUM(G11:G14)/SUM(K11:K14) * K10</f>
         <v>10.125</v>
       </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="3">
-        <f>IF(ISBLANK(H9),G9,H9)</f>
+      <c r="H10" s="11"/>
+      <c r="I10" s="3">
+        <f>IF(ISBLANK(H10),G10,H10)</f>
         <v>10.125</v>
       </c>
-      <c r="J9" t="s">
-        <v>34</v>
-      </c>
-      <c r="K9">
+      <c r="J10" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10">
         <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="E10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="13">
-        <f>IF(IF(ISBLANK(B10),0,1) + IF(ISBLANK(C10),0,1) + IF(ISBLANK(D10),0,1) + IF(ISBLANK(E10),0,1) + IF(ISBLANK(F10),0,1) = 1,IF(IF(ISBLANK(B10),0,IF(ISNUMBER(B10),B10,K10)) + IF(ISBLANK(C10),0,IF(ISNUMBER(C10),C10,L10)) + IF(ISBLANK(D10),0,IF(ISNUMBER(D10),D10,M10)) + IF(ISBLANK(E10),0,IF(ISNUMBER(E10),E10,N10)) + IF(ISBLANK(F10),0,IF(ISNUMBER(F10),F10,O10)) &gt; K10, NA(), IF(ISBLANK(B10),0,IF(ISNUMBER(B10),B10,K10)) + IF(ISBLANK(C10),0,IF(ISNUMBER(C10),C10,L10)) + IF(ISBLANK(D10),0,IF(ISNUMBER(D10),D10,M10)) + IF(ISBLANK(E10),0,IF(ISNUMBER(E10),E10,N10)) + IF(ISBLANK(F10),0,IF(ISNUMBER(F10),F10,O10))),NA())</f>
-        <v>13</v>
-      </c>
-      <c r="K10" s="12">
-        <v>20</v>
-      </c>
-      <c r="L10" s="12">
-        <v>17</v>
-      </c>
-      <c r="M10" s="12">
-        <v>15</v>
-      </c>
-      <c r="N10" s="12">
-        <v>13</v>
-      </c>
-      <c r="O10" s="12">
-        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="16" x14ac:dyDescent="0.2">
@@ -1792,12 +1812,12 @@
         <v>18</v>
       </c>
       <c r="B11" s="12"/>
-      <c r="D11" t="s">
-        <v>33</v>
+      <c r="E11" t="s">
+        <v>34</v>
       </c>
       <c r="G11" s="13">
         <f>IF(IF(ISBLANK(B11),0,1) + IF(ISBLANK(C11),0,1) + IF(ISBLANK(D11),0,1) + IF(ISBLANK(E11),0,1) + IF(ISBLANK(F11),0,1) = 1,IF(IF(ISBLANK(B11),0,IF(ISNUMBER(B11),B11,K11)) + IF(ISBLANK(C11),0,IF(ISNUMBER(C11),C11,L11)) + IF(ISBLANK(D11),0,IF(ISNUMBER(D11),D11,M11)) + IF(ISBLANK(E11),0,IF(ISNUMBER(E11),E11,N11)) + IF(ISBLANK(F11),0,IF(ISNUMBER(F11),F11,O11)) &gt; K11, NA(), IF(ISBLANK(B11),0,IF(ISNUMBER(B11),B11,K11)) + IF(ISBLANK(C11),0,IF(ISNUMBER(C11),C11,L11)) + IF(ISBLANK(D11),0,IF(ISNUMBER(D11),D11,M11)) + IF(ISBLANK(E11),0,IF(ISNUMBER(E11),E11,N11)) + IF(ISBLANK(F11),0,IF(ISNUMBER(F11),F11,O11))),NA())</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K11" s="12">
         <v>20</v>
@@ -1821,7 +1841,7 @@
       </c>
       <c r="B12" s="12"/>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G12" s="13">
         <f>IF(IF(ISBLANK(B12),0,1) + IF(ISBLANK(C12),0,1) + IF(ISBLANK(D12),0,1) + IF(ISBLANK(E12),0,1) + IF(ISBLANK(F12),0,1) = 1,IF(IF(ISBLANK(B12),0,IF(ISNUMBER(B12),B12,K12)) + IF(ISBLANK(C12),0,IF(ISNUMBER(C12),C12,L12)) + IF(ISBLANK(D12),0,IF(ISNUMBER(D12),D12,M12)) + IF(ISBLANK(E12),0,IF(ISNUMBER(E12),E12,N12)) + IF(ISBLANK(F12),0,IF(ISNUMBER(F12),F12,O12)) &gt; K12, NA(), IF(ISBLANK(B12),0,IF(ISNUMBER(B12),B12,K12)) + IF(ISBLANK(C12),0,IF(ISNUMBER(C12),C12,L12)) + IF(ISBLANK(D12),0,IF(ISNUMBER(D12),D12,M12)) + IF(ISBLANK(E12),0,IF(ISNUMBER(E12),E12,N12)) + IF(ISBLANK(F12),0,IF(ISNUMBER(F12),F12,O12))),NA())</f>
@@ -1848,12 +1868,12 @@
         <v>20</v>
       </c>
       <c r="B13" s="12"/>
-      <c r="F13" t="s">
-        <v>33</v>
+      <c r="D13" t="s">
+        <v>34</v>
       </c>
       <c r="G13" s="13">
         <f>IF(IF(ISBLANK(B13),0,1) + IF(ISBLANK(C13),0,1) + IF(ISBLANK(D13),0,1) + IF(ISBLANK(E13),0,1) + IF(ISBLANK(F13),0,1) = 1,IF(IF(ISBLANK(B13),0,IF(ISNUMBER(B13),B13,K13)) + IF(ISBLANK(C13),0,IF(ISNUMBER(C13),C13,L13)) + IF(ISBLANK(D13),0,IF(ISNUMBER(D13),D13,M13)) + IF(ISBLANK(E13),0,IF(ISNUMBER(E13),E13,N13)) + IF(ISBLANK(F13),0,IF(ISNUMBER(F13),F13,O13)) &gt; K13, NA(), IF(ISBLANK(B13),0,IF(ISNUMBER(B13),B13,K13)) + IF(ISBLANK(C13),0,IF(ISNUMBER(C13),C13,L13)) + IF(ISBLANK(D13),0,IF(ISNUMBER(D13),D13,M13)) + IF(ISBLANK(E13),0,IF(ISNUMBER(E13),E13,N13)) + IF(ISBLANK(F13),0,IF(ISNUMBER(F13),F13,O13))),NA())</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="K13" s="12">
         <v>20</v>
@@ -1872,51 +1892,51 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="3">
-        <f>SUM(G15:G17)/SUM(K15:K17) * K14</f>
+      <c r="B14" s="12"/>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="13">
+        <f>IF(IF(ISBLANK(B14),0,1) + IF(ISBLANK(C14),0,1) + IF(ISBLANK(D14),0,1) + IF(ISBLANK(E14),0,1) + IF(ISBLANK(F14),0,1) = 1,IF(IF(ISBLANK(B14),0,IF(ISNUMBER(B14),B14,K14)) + IF(ISBLANK(C14),0,IF(ISNUMBER(C14),C14,L14)) + IF(ISBLANK(D14),0,IF(ISNUMBER(D14),D14,M14)) + IF(ISBLANK(E14),0,IF(ISNUMBER(E14),E14,N14)) + IF(ISBLANK(F14),0,IF(ISNUMBER(F14),F14,O14)) &gt; K14, NA(), IF(ISBLANK(B14),0,IF(ISNUMBER(B14),B14,K14)) + IF(ISBLANK(C14),0,IF(ISNUMBER(C14),C14,L14)) + IF(ISBLANK(D14),0,IF(ISNUMBER(D14),D14,M14)) + IF(ISBLANK(E14),0,IF(ISNUMBER(E14),E14,N14)) + IF(ISBLANK(F14),0,IF(ISNUMBER(F14),F14,O14))),NA())</f>
+        <v>11</v>
+      </c>
+      <c r="K14" s="12">
+        <v>20</v>
+      </c>
+      <c r="L14" s="12">
+        <v>17</v>
+      </c>
+      <c r="M14" s="12">
+        <v>15</v>
+      </c>
+      <c r="N14" s="12">
+        <v>13</v>
+      </c>
+      <c r="O14" s="12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="3">
+        <f>SUM(G16:G18)/SUM(K16:K18) * K15</f>
         <v>8</v>
       </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="3">
-        <f>IF(ISBLANK(H14),G14,H14)</f>
+      <c r="H15" s="11"/>
+      <c r="I15" s="3">
+        <f>IF(ISBLANK(H15),G15,H15)</f>
         <v>8</v>
       </c>
-      <c r="J14" t="s">
-        <v>35</v>
-      </c>
-      <c r="K14">
+      <c r="J15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15">
         <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="12"/>
-      <c r="F15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="13">
-        <f>IF(IF(ISBLANK(B15),0,1) + IF(ISBLANK(C15),0,1) + IF(ISBLANK(D15),0,1) + IF(ISBLANK(E15),0,1) + IF(ISBLANK(F15),0,1) = 1,IF(IF(ISBLANK(B15),0,IF(ISNUMBER(B15),B15,K15)) + IF(ISBLANK(C15),0,IF(ISNUMBER(C15),C15,L15)) + IF(ISBLANK(D15),0,IF(ISNUMBER(D15),D15,M15)) + IF(ISBLANK(E15),0,IF(ISNUMBER(E15),E15,N15)) + IF(ISBLANK(F15),0,IF(ISNUMBER(F15),F15,O15)) &gt; K15, NA(), IF(ISBLANK(B15),0,IF(ISNUMBER(B15),B15,K15)) + IF(ISBLANK(C15),0,IF(ISNUMBER(C15),C15,L15)) + IF(ISBLANK(D15),0,IF(ISNUMBER(D15),D15,M15)) + IF(ISBLANK(E15),0,IF(ISNUMBER(E15),E15,N15)) + IF(ISBLANK(F15),0,IF(ISNUMBER(F15),F15,O15))),NA())</f>
-        <v>0</v>
-      </c>
-      <c r="K15" s="12">
-        <v>5</v>
-      </c>
-      <c r="L15" s="12">
-        <v>4</v>
-      </c>
-      <c r="M15" s="12">
-        <v>3</v>
-      </c>
-      <c r="N15" s="12">
-        <v>2</v>
-      </c>
-      <c r="O15" s="12">
-        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="16" x14ac:dyDescent="0.2">
@@ -1924,12 +1944,12 @@
         <v>23</v>
       </c>
       <c r="B16" s="12"/>
-      <c r="D16" t="s">
-        <v>33</v>
+      <c r="F16" t="s">
+        <v>34</v>
       </c>
       <c r="G16" s="13">
         <f>IF(IF(ISBLANK(B16),0,1) + IF(ISBLANK(C16),0,1) + IF(ISBLANK(D16),0,1) + IF(ISBLANK(E16),0,1) + IF(ISBLANK(F16),0,1) = 1,IF(IF(ISBLANK(B16),0,IF(ISNUMBER(B16),B16,K16)) + IF(ISBLANK(C16),0,IF(ISNUMBER(C16),C16,L16)) + IF(ISBLANK(D16),0,IF(ISNUMBER(D16),D16,M16)) + IF(ISBLANK(E16),0,IF(ISNUMBER(E16),E16,N16)) + IF(ISBLANK(F16),0,IF(ISNUMBER(F16),F16,O16)) &gt; K16, NA(), IF(ISBLANK(B16),0,IF(ISNUMBER(B16),B16,K16)) + IF(ISBLANK(C16),0,IF(ISNUMBER(C16),C16,L16)) + IF(ISBLANK(D16),0,IF(ISNUMBER(D16),D16,M16)) + IF(ISBLANK(E16),0,IF(ISNUMBER(E16),E16,N16)) + IF(ISBLANK(F16),0,IF(ISNUMBER(F16),F16,O16))),NA())</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K16" s="12">
         <v>5</v>
@@ -1953,7 +1973,7 @@
       </c>
       <c r="B17" s="12"/>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G17" s="13">
         <f>IF(IF(ISBLANK(B17),0,1) + IF(ISBLANK(C17),0,1) + IF(ISBLANK(D17),0,1) + IF(ISBLANK(E17),0,1) + IF(ISBLANK(F17),0,1) = 1,IF(IF(ISBLANK(B17),0,IF(ISNUMBER(B17),B17,K17)) + IF(ISBLANK(C17),0,IF(ISNUMBER(C17),C17,L17)) + IF(ISBLANK(D17),0,IF(ISNUMBER(D17),D17,M17)) + IF(ISBLANK(E17),0,IF(ISNUMBER(E17),E17,N17)) + IF(ISBLANK(F17),0,IF(ISNUMBER(F17),F17,O17)) &gt; K17, NA(), IF(ISBLANK(B17),0,IF(ISNUMBER(B17),B17,K17)) + IF(ISBLANK(C17),0,IF(ISNUMBER(C17),C17,L17)) + IF(ISBLANK(D17),0,IF(ISNUMBER(D17),D17,M17)) + IF(ISBLANK(E17),0,IF(ISNUMBER(E17),E17,N17)) + IF(ISBLANK(F17),0,IF(ISNUMBER(F17),F17,O17))),NA())</f>
@@ -1976,51 +1996,51 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="3">
-        <f>SUM(G19:G21)/SUM(K19:K21) * K18</f>
+      <c r="B18" s="12"/>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="13">
+        <f>IF(IF(ISBLANK(B18),0,1) + IF(ISBLANK(C18),0,1) + IF(ISBLANK(D18),0,1) + IF(ISBLANK(E18),0,1) + IF(ISBLANK(F18),0,1) = 1,IF(IF(ISBLANK(B18),0,IF(ISNUMBER(B18),B18,K18)) + IF(ISBLANK(C18),0,IF(ISNUMBER(C18),C18,L18)) + IF(ISBLANK(D18),0,IF(ISNUMBER(D18),D18,M18)) + IF(ISBLANK(E18),0,IF(ISNUMBER(E18),E18,N18)) + IF(ISBLANK(F18),0,IF(ISNUMBER(F18),F18,O18)) &gt; K18, NA(), IF(ISBLANK(B18),0,IF(ISNUMBER(B18),B18,K18)) + IF(ISBLANK(C18),0,IF(ISNUMBER(C18),C18,L18)) + IF(ISBLANK(D18),0,IF(ISNUMBER(D18),D18,M18)) + IF(ISBLANK(E18),0,IF(ISNUMBER(E18),E18,N18)) + IF(ISBLANK(F18),0,IF(ISNUMBER(F18),F18,O18))),NA())</f>
+        <v>3</v>
+      </c>
+      <c r="K18" s="12">
+        <v>5</v>
+      </c>
+      <c r="L18" s="12">
+        <v>4</v>
+      </c>
+      <c r="M18" s="12">
+        <v>3</v>
+      </c>
+      <c r="N18" s="12">
+        <v>2</v>
+      </c>
+      <c r="O18" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="3">
+        <f>SUM(G20:G22)/SUM(K20:K22) * K19</f>
         <v>9.5</v>
       </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="3">
-        <f>IF(ISBLANK(H18),G18,H18)</f>
+      <c r="H19" s="11"/>
+      <c r="I19" s="3">
+        <f>IF(ISBLANK(H19),G19,H19)</f>
         <v>9.5</v>
       </c>
-      <c r="J18" t="s">
-        <v>36</v>
-      </c>
-      <c r="K18">
+      <c r="J19" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19">
         <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="12"/>
-      <c r="D19" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="13">
-        <f>IF(IF(ISBLANK(B19),0,1) + IF(ISBLANK(C19),0,1) + IF(ISBLANK(D19),0,1) + IF(ISBLANK(E19),0,1) + IF(ISBLANK(F19),0,1) = 1,IF(IF(ISBLANK(B19),0,IF(ISNUMBER(B19),B19,K19)) + IF(ISBLANK(C19),0,IF(ISNUMBER(C19),C19,L19)) + IF(ISBLANK(D19),0,IF(ISNUMBER(D19),D19,M19)) + IF(ISBLANK(E19),0,IF(ISNUMBER(E19),E19,N19)) + IF(ISBLANK(F19),0,IF(ISNUMBER(F19),F19,O19)) &gt; K19, NA(), IF(ISBLANK(B19),0,IF(ISNUMBER(B19),B19,K19)) + IF(ISBLANK(C19),0,IF(ISNUMBER(C19),C19,L19)) + IF(ISBLANK(D19),0,IF(ISNUMBER(D19),D19,M19)) + IF(ISBLANK(E19),0,IF(ISNUMBER(E19),E19,N19)) + IF(ISBLANK(F19),0,IF(ISNUMBER(F19),F19,O19))),NA())</f>
-        <v>3</v>
-      </c>
-      <c r="K19" s="12">
-        <v>5</v>
-      </c>
-      <c r="L19" s="12">
-        <v>4</v>
-      </c>
-      <c r="M19" s="12">
-        <v>3</v>
-      </c>
-      <c r="N19" s="12">
-        <v>2</v>
-      </c>
-      <c r="O19" s="12">
-        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="16" x14ac:dyDescent="0.2">
@@ -2029,7 +2049,7 @@
       </c>
       <c r="B20" s="12"/>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G20" s="13">
         <f>IF(IF(ISBLANK(B20),0,1) + IF(ISBLANK(C20),0,1) + IF(ISBLANK(D20),0,1) + IF(ISBLANK(E20),0,1) + IF(ISBLANK(F20),0,1) = 1,IF(IF(ISBLANK(B20),0,IF(ISNUMBER(B20),B20,K20)) + IF(ISBLANK(C20),0,IF(ISNUMBER(C20),C20,L20)) + IF(ISBLANK(D20),0,IF(ISNUMBER(D20),D20,M20)) + IF(ISBLANK(E20),0,IF(ISNUMBER(E20),E20,N20)) + IF(ISBLANK(F20),0,IF(ISNUMBER(F20),F20,O20)) &gt; K20, NA(), IF(ISBLANK(B20),0,IF(ISNUMBER(B20),B20,K20)) + IF(ISBLANK(C20),0,IF(ISNUMBER(C20),C20,L20)) + IF(ISBLANK(D20),0,IF(ISNUMBER(D20),D20,M20)) + IF(ISBLANK(E20),0,IF(ISNUMBER(E20),E20,N20)) + IF(ISBLANK(F20),0,IF(ISNUMBER(F20),F20,O20))),NA())</f>
@@ -2056,103 +2076,131 @@
         <v>28</v>
       </c>
       <c r="B21" s="12"/>
-      <c r="E21" t="s">
-        <v>33</v>
+      <c r="D21" t="s">
+        <v>34</v>
       </c>
       <c r="G21" s="13">
         <f>IF(IF(ISBLANK(B21),0,1) + IF(ISBLANK(C21),0,1) + IF(ISBLANK(D21),0,1) + IF(ISBLANK(E21),0,1) + IF(ISBLANK(F21),0,1) = 1,IF(IF(ISBLANK(B21),0,IF(ISNUMBER(B21),B21,K21)) + IF(ISBLANK(C21),0,IF(ISNUMBER(C21),C21,L21)) + IF(ISBLANK(D21),0,IF(ISNUMBER(D21),D21,M21)) + IF(ISBLANK(E21),0,IF(ISNUMBER(E21),E21,N21)) + IF(ISBLANK(F21),0,IF(ISNUMBER(F21),F21,O21)) &gt; K21, NA(), IF(ISBLANK(B21),0,IF(ISNUMBER(B21),B21,K21)) + IF(ISBLANK(C21),0,IF(ISNUMBER(C21),C21,L21)) + IF(ISBLANK(D21),0,IF(ISNUMBER(D21),D21,M21)) + IF(ISBLANK(E21),0,IF(ISNUMBER(E21),E21,N21)) + IF(ISBLANK(F21),0,IF(ISNUMBER(F21),F21,O21))),NA())</f>
+        <v>3</v>
+      </c>
+      <c r="K21" s="12">
+        <v>5</v>
+      </c>
+      <c r="L21" s="12">
+        <v>4</v>
+      </c>
+      <c r="M21" s="12">
+        <v>3</v>
+      </c>
+      <c r="N21" s="12">
+        <v>2</v>
+      </c>
+      <c r="O21" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="13">
+        <f>IF(IF(ISBLANK(B22),0,1) + IF(ISBLANK(C22),0,1) + IF(ISBLANK(D22),0,1) + IF(ISBLANK(E22),0,1) + IF(ISBLANK(F22),0,1) = 1,IF(IF(ISBLANK(B22),0,IF(ISNUMBER(B22),B22,K22)) + IF(ISBLANK(C22),0,IF(ISNUMBER(C22),C22,L22)) + IF(ISBLANK(D22),0,IF(ISNUMBER(D22),D22,M22)) + IF(ISBLANK(E22),0,IF(ISNUMBER(E22),E22,N22)) + IF(ISBLANK(F22),0,IF(ISNUMBER(F22),F22,O22)) &gt; K22, NA(), IF(ISBLANK(B22),0,IF(ISNUMBER(B22),B22,K22)) + IF(ISBLANK(C22),0,IF(ISNUMBER(C22),C22,L22)) + IF(ISBLANK(D22),0,IF(ISNUMBER(D22),D22,M22)) + IF(ISBLANK(E22),0,IF(ISNUMBER(E22),E22,N22)) + IF(ISBLANK(F22),0,IF(ISNUMBER(F22),F22,O22))),NA())</f>
         <v>13</v>
       </c>
-      <c r="K21" s="12">
+      <c r="K22" s="12">
         <v>20</v>
       </c>
-      <c r="L21" s="12">
+      <c r="L22" s="12">
         <v>17</v>
       </c>
-      <c r="M21" s="12">
+      <c r="M22" s="12">
         <v>15</v>
       </c>
-      <c r="N21" s="12">
+      <c r="N22" s="12">
         <v>13</v>
       </c>
-      <c r="O21" s="12">
+      <c r="O22" s="12">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B10:B13">
-    <cfRule type="expression" dxfId="29" priority="1" stopIfTrue="1">
-      <formula>NOT(ISBLANK(B10))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15:B17">
-    <cfRule type="expression" dxfId="28" priority="21" stopIfTrue="1">
-      <formula>NOT(ISBLANK(B15))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19:B21">
-    <cfRule type="expression" dxfId="27" priority="36" stopIfTrue="1">
-      <formula>NOT(ISBLANK(B19))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10:C13">
-    <cfRule type="expression" dxfId="26" priority="2" stopIfTrue="1">
-      <formula>NOT(ISBLANK(C10))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15:C17">
-    <cfRule type="expression" dxfId="25" priority="22" stopIfTrue="1">
-      <formula>NOT(ISBLANK(C15))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19:C21">
-    <cfRule type="expression" dxfId="24" priority="37" stopIfTrue="1">
-      <formula>NOT(ISBLANK(C19))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D10:D13">
-    <cfRule type="expression" dxfId="23" priority="3" stopIfTrue="1">
-      <formula>NOT(ISBLANK(D10))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D15:D17">
-    <cfRule type="expression" dxfId="22" priority="23" stopIfTrue="1">
-      <formula>NOT(ISBLANK(D15))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D19:D21">
-    <cfRule type="expression" dxfId="21" priority="38" stopIfTrue="1">
-      <formula>NOT(ISBLANK(D19))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E10:E13">
-    <cfRule type="expression" dxfId="20" priority="4" stopIfTrue="1">
-      <formula>NOT(ISBLANK(E10))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E15:E17">
-    <cfRule type="expression" dxfId="19" priority="24" stopIfTrue="1">
-      <formula>NOT(ISBLANK(E15))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E19:E21">
-    <cfRule type="expression" dxfId="18" priority="39" stopIfTrue="1">
-      <formula>NOT(ISBLANK(E19))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F10:F13">
-    <cfRule type="expression" dxfId="17" priority="5" stopIfTrue="1">
-      <formula>NOT(ISBLANK(F10))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F15:F17">
-    <cfRule type="expression" dxfId="16" priority="25" stopIfTrue="1">
-      <formula>NOT(ISBLANK(F15))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F19:F21">
-    <cfRule type="expression" dxfId="15" priority="40" stopIfTrue="1">
-      <formula>NOT(ISBLANK(F19))</formula>
+  <conditionalFormatting sqref="B11:B14">
+    <cfRule type="expression" dxfId="32" priority="1" stopIfTrue="1">
+      <formula>NOT(ISBLANK(B11))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16:B18">
+    <cfRule type="expression" dxfId="31" priority="21" stopIfTrue="1">
+      <formula>NOT(ISBLANK(B16))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20:B22">
+    <cfRule type="expression" dxfId="30" priority="36" stopIfTrue="1">
+      <formula>NOT(ISBLANK(B20))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:C14">
+    <cfRule type="expression" dxfId="29" priority="2" stopIfTrue="1">
+      <formula>NOT(ISBLANK(C11))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16:C18">
+    <cfRule type="expression" dxfId="28" priority="22" stopIfTrue="1">
+      <formula>NOT(ISBLANK(C16))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20:C22">
+    <cfRule type="expression" dxfId="27" priority="37" stopIfTrue="1">
+      <formula>NOT(ISBLANK(C20))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11:D14">
+    <cfRule type="expression" dxfId="26" priority="3" stopIfTrue="1">
+      <formula>NOT(ISBLANK(D11))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:D18">
+    <cfRule type="expression" dxfId="25" priority="23" stopIfTrue="1">
+      <formula>NOT(ISBLANK(D16))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20:D22">
+    <cfRule type="expression" dxfId="24" priority="38" stopIfTrue="1">
+      <formula>NOT(ISBLANK(D20))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11:E14">
+    <cfRule type="expression" dxfId="23" priority="4" stopIfTrue="1">
+      <formula>NOT(ISBLANK(E11))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16:E18">
+    <cfRule type="expression" dxfId="22" priority="24" stopIfTrue="1">
+      <formula>NOT(ISBLANK(E16))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20:E22">
+    <cfRule type="expression" dxfId="21" priority="39" stopIfTrue="1">
+      <formula>NOT(ISBLANK(E20))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11:F14">
+    <cfRule type="expression" dxfId="20" priority="5" stopIfTrue="1">
+      <formula>NOT(ISBLANK(F11))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16:F18">
+    <cfRule type="expression" dxfId="19" priority="25" stopIfTrue="1">
+      <formula>NOT(ISBLANK(F16))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20:F22">
+    <cfRule type="expression" dxfId="18" priority="40" stopIfTrue="1">
+      <formula>NOT(ISBLANK(F20))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2161,10 +2209,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2185,7 +2233,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -2193,93 +2241,73 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
-        <f>SUM(I9,I14,I18)</f>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <f>SUM(I10,I15,I19)</f>
         <v>41.25</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="5" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="F9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="H9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="I9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="J9" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="K9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="3">
-        <f>SUM(G10:G13)/SUM(K10:K13) * K9</f>
+    </row>
+    <row r="10" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="3">
+        <f>SUM(G11:G14)/SUM(K11:K14) * K10</f>
         <v>12.75</v>
       </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="3">
-        <f>IF(ISBLANK(H9),G9,H9)</f>
+      <c r="H10" s="11"/>
+      <c r="I10" s="3">
+        <f>IF(ISBLANK(H10),G10,H10)</f>
         <v>12.75</v>
       </c>
-      <c r="K9">
+      <c r="K10">
         <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="13">
-        <f>IF(IF(ISBLANK(B10),0,1) + IF(ISBLANK(C10),0,1) + IF(ISBLANK(D10),0,1) + IF(ISBLANK(E10),0,1) + IF(ISBLANK(F10),0,1) = 1,IF(IF(ISBLANK(B10),0,IF(ISNUMBER(B10),B10,K10)) + IF(ISBLANK(C10),0,IF(ISNUMBER(C10),C10,L10)) + IF(ISBLANK(D10),0,IF(ISNUMBER(D10),D10,M10)) + IF(ISBLANK(E10),0,IF(ISNUMBER(E10),E10,N10)) + IF(ISBLANK(F10),0,IF(ISNUMBER(F10),F10,O10)) &gt; K10, NA(), IF(ISBLANK(B10),0,IF(ISNUMBER(B10),B10,K10)) + IF(ISBLANK(C10),0,IF(ISNUMBER(C10),C10,L10)) + IF(ISBLANK(D10),0,IF(ISNUMBER(D10),D10,M10)) + IF(ISBLANK(E10),0,IF(ISNUMBER(E10),E10,N10)) + IF(ISBLANK(F10),0,IF(ISNUMBER(F10),F10,O10))),NA())</f>
-        <v>17</v>
-      </c>
-      <c r="K10" s="12">
-        <v>20</v>
-      </c>
-      <c r="L10" s="12">
-        <v>17</v>
-      </c>
-      <c r="M10" s="12">
-        <v>15</v>
-      </c>
-      <c r="N10" s="12">
-        <v>13</v>
-      </c>
-      <c r="O10" s="12">
-        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="16" x14ac:dyDescent="0.2">
@@ -2288,7 +2316,7 @@
       </c>
       <c r="B11" s="12"/>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G11" s="13">
         <f>IF(IF(ISBLANK(B11),0,1) + IF(ISBLANK(C11),0,1) + IF(ISBLANK(D11),0,1) + IF(ISBLANK(E11),0,1) + IF(ISBLANK(F11),0,1) = 1,IF(IF(ISBLANK(B11),0,IF(ISNUMBER(B11),B11,K11)) + IF(ISBLANK(C11),0,IF(ISNUMBER(C11),C11,L11)) + IF(ISBLANK(D11),0,IF(ISNUMBER(D11),D11,M11)) + IF(ISBLANK(E11),0,IF(ISNUMBER(E11),E11,N11)) + IF(ISBLANK(F11),0,IF(ISNUMBER(F11),F11,O11)) &gt; K11, NA(), IF(ISBLANK(B11),0,IF(ISNUMBER(B11),B11,K11)) + IF(ISBLANK(C11),0,IF(ISNUMBER(C11),C11,L11)) + IF(ISBLANK(D11),0,IF(ISNUMBER(D11),D11,M11)) + IF(ISBLANK(E11),0,IF(ISNUMBER(E11),E11,N11)) + IF(ISBLANK(F11),0,IF(ISNUMBER(F11),F11,O11))),NA())</f>
@@ -2316,7 +2344,7 @@
       </c>
       <c r="B12" s="12"/>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G12" s="13">
         <f>IF(IF(ISBLANK(B12),0,1) + IF(ISBLANK(C12),0,1) + IF(ISBLANK(D12),0,1) + IF(ISBLANK(E12),0,1) + IF(ISBLANK(F12),0,1) = 1,IF(IF(ISBLANK(B12),0,IF(ISNUMBER(B12),B12,K12)) + IF(ISBLANK(C12),0,IF(ISNUMBER(C12),C12,L12)) + IF(ISBLANK(D12),0,IF(ISNUMBER(D12),D12,M12)) + IF(ISBLANK(E12),0,IF(ISNUMBER(E12),E12,N12)) + IF(ISBLANK(F12),0,IF(ISNUMBER(F12),F12,O12)) &gt; K12, NA(), IF(ISBLANK(B12),0,IF(ISNUMBER(B12),B12,K12)) + IF(ISBLANK(C12),0,IF(ISNUMBER(C12),C12,L12)) + IF(ISBLANK(D12),0,IF(ISNUMBER(D12),D12,M12)) + IF(ISBLANK(E12),0,IF(ISNUMBER(E12),E12,N12)) + IF(ISBLANK(F12),0,IF(ISNUMBER(F12),F12,O12))),NA())</f>
@@ -2344,7 +2372,7 @@
       </c>
       <c r="B13" s="12"/>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G13" s="13">
         <f>IF(IF(ISBLANK(B13),0,1) + IF(ISBLANK(C13),0,1) + IF(ISBLANK(D13),0,1) + IF(ISBLANK(E13),0,1) + IF(ISBLANK(F13),0,1) = 1,IF(IF(ISBLANK(B13),0,IF(ISNUMBER(B13),B13,K13)) + IF(ISBLANK(C13),0,IF(ISNUMBER(C13),C13,L13)) + IF(ISBLANK(D13),0,IF(ISNUMBER(D13),D13,M13)) + IF(ISBLANK(E13),0,IF(ISNUMBER(E13),E13,N13)) + IF(ISBLANK(F13),0,IF(ISNUMBER(F13),F13,O13)) &gt; K13, NA(), IF(ISBLANK(B13),0,IF(ISNUMBER(B13),B13,K13)) + IF(ISBLANK(C13),0,IF(ISNUMBER(C13),C13,L13)) + IF(ISBLANK(D13),0,IF(ISNUMBER(D13),D13,M13)) + IF(ISBLANK(E13),0,IF(ISNUMBER(E13),E13,N13)) + IF(ISBLANK(F13),0,IF(ISNUMBER(F13),F13,O13))),NA())</f>
@@ -2367,48 +2395,48 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="3">
-        <f>SUM(G15:G17)/SUM(K15:K17) * K14</f>
+      <c r="B14" s="12"/>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="13">
+        <f>IF(IF(ISBLANK(B14),0,1) + IF(ISBLANK(C14),0,1) + IF(ISBLANK(D14),0,1) + IF(ISBLANK(E14),0,1) + IF(ISBLANK(F14),0,1) = 1,IF(IF(ISBLANK(B14),0,IF(ISNUMBER(B14),B14,K14)) + IF(ISBLANK(C14),0,IF(ISNUMBER(C14),C14,L14)) + IF(ISBLANK(D14),0,IF(ISNUMBER(D14),D14,M14)) + IF(ISBLANK(E14),0,IF(ISNUMBER(E14),E14,N14)) + IF(ISBLANK(F14),0,IF(ISNUMBER(F14),F14,O14)) &gt; K14, NA(), IF(ISBLANK(B14),0,IF(ISNUMBER(B14),B14,K14)) + IF(ISBLANK(C14),0,IF(ISNUMBER(C14),C14,L14)) + IF(ISBLANK(D14),0,IF(ISNUMBER(D14),D14,M14)) + IF(ISBLANK(E14),0,IF(ISNUMBER(E14),E14,N14)) + IF(ISBLANK(F14),0,IF(ISNUMBER(F14),F14,O14))),NA())</f>
+        <v>17</v>
+      </c>
+      <c r="K14" s="12">
+        <v>20</v>
+      </c>
+      <c r="L14" s="12">
+        <v>17</v>
+      </c>
+      <c r="M14" s="12">
+        <v>15</v>
+      </c>
+      <c r="N14" s="12">
+        <v>13</v>
+      </c>
+      <c r="O14" s="12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="3">
+        <f>SUM(G16:G18)/SUM(K16:K18) * K15</f>
         <v>16</v>
       </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="3">
-        <f>IF(ISBLANK(H14),G14,H14)</f>
+      <c r="H15" s="11"/>
+      <c r="I15" s="3">
+        <f>IF(ISBLANK(H15),G15,H15)</f>
         <v>16</v>
       </c>
-      <c r="K14">
+      <c r="K15">
         <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="12"/>
-      <c r="C15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="13">
-        <f>IF(IF(ISBLANK(B15),0,1) + IF(ISBLANK(C15),0,1) + IF(ISBLANK(D15),0,1) + IF(ISBLANK(E15),0,1) + IF(ISBLANK(F15),0,1) = 1,IF(IF(ISBLANK(B15),0,IF(ISNUMBER(B15),B15,K15)) + IF(ISBLANK(C15),0,IF(ISNUMBER(C15),C15,L15)) + IF(ISBLANK(D15),0,IF(ISNUMBER(D15),D15,M15)) + IF(ISBLANK(E15),0,IF(ISNUMBER(E15),E15,N15)) + IF(ISBLANK(F15),0,IF(ISNUMBER(F15),F15,O15)) &gt; K15, NA(), IF(ISBLANK(B15),0,IF(ISNUMBER(B15),B15,K15)) + IF(ISBLANK(C15),0,IF(ISNUMBER(C15),C15,L15)) + IF(ISBLANK(D15),0,IF(ISNUMBER(D15),D15,M15)) + IF(ISBLANK(E15),0,IF(ISNUMBER(E15),E15,N15)) + IF(ISBLANK(F15),0,IF(ISNUMBER(F15),F15,O15))),NA())</f>
-        <v>4</v>
-      </c>
-      <c r="K15" s="12">
-        <v>5</v>
-      </c>
-      <c r="L15" s="12">
-        <v>4</v>
-      </c>
-      <c r="M15" s="12">
-        <v>3</v>
-      </c>
-      <c r="N15" s="12">
-        <v>2</v>
-      </c>
-      <c r="O15" s="12">
-        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="16" x14ac:dyDescent="0.2">
@@ -2417,7 +2445,7 @@
       </c>
       <c r="B16" s="12"/>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G16" s="13">
         <f>IF(IF(ISBLANK(B16),0,1) + IF(ISBLANK(C16),0,1) + IF(ISBLANK(D16),0,1) + IF(ISBLANK(E16),0,1) + IF(ISBLANK(F16),0,1) = 1,IF(IF(ISBLANK(B16),0,IF(ISNUMBER(B16),B16,K16)) + IF(ISBLANK(C16),0,IF(ISNUMBER(C16),C16,L16)) + IF(ISBLANK(D16),0,IF(ISNUMBER(D16),D16,M16)) + IF(ISBLANK(E16),0,IF(ISNUMBER(E16),E16,N16)) + IF(ISBLANK(F16),0,IF(ISNUMBER(F16),F16,O16)) &gt; K16, NA(), IF(ISBLANK(B16),0,IF(ISNUMBER(B16),B16,K16)) + IF(ISBLANK(C16),0,IF(ISNUMBER(C16),C16,L16)) + IF(ISBLANK(D16),0,IF(ISNUMBER(D16),D16,M16)) + IF(ISBLANK(E16),0,IF(ISNUMBER(E16),E16,N16)) + IF(ISBLANK(F16),0,IF(ISNUMBER(F16),F16,O16))),NA())</f>
@@ -2445,7 +2473,7 @@
       </c>
       <c r="B17" s="12"/>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G17" s="13">
         <f>IF(IF(ISBLANK(B17),0,1) + IF(ISBLANK(C17),0,1) + IF(ISBLANK(D17),0,1) + IF(ISBLANK(E17),0,1) + IF(ISBLANK(F17),0,1) = 1,IF(IF(ISBLANK(B17),0,IF(ISNUMBER(B17),B17,K17)) + IF(ISBLANK(C17),0,IF(ISNUMBER(C17),C17,L17)) + IF(ISBLANK(D17),0,IF(ISNUMBER(D17),D17,M17)) + IF(ISBLANK(E17),0,IF(ISNUMBER(E17),E17,N17)) + IF(ISBLANK(F17),0,IF(ISNUMBER(F17),F17,O17)) &gt; K17, NA(), IF(ISBLANK(B17),0,IF(ISNUMBER(B17),B17,K17)) + IF(ISBLANK(C17),0,IF(ISNUMBER(C17),C17,L17)) + IF(ISBLANK(D17),0,IF(ISNUMBER(D17),D17,M17)) + IF(ISBLANK(E17),0,IF(ISNUMBER(E17),E17,N17)) + IF(ISBLANK(F17),0,IF(ISNUMBER(F17),F17,O17))),NA())</f>
@@ -2468,48 +2496,48 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="3">
-        <f>SUM(G19:G21)/SUM(K19:K21) * K18</f>
+      <c r="B18" s="12"/>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="13">
+        <f>IF(IF(ISBLANK(B18),0,1) + IF(ISBLANK(C18),0,1) + IF(ISBLANK(D18),0,1) + IF(ISBLANK(E18),0,1) + IF(ISBLANK(F18),0,1) = 1,IF(IF(ISBLANK(B18),0,IF(ISNUMBER(B18),B18,K18)) + IF(ISBLANK(C18),0,IF(ISNUMBER(C18),C18,L18)) + IF(ISBLANK(D18),0,IF(ISNUMBER(D18),D18,M18)) + IF(ISBLANK(E18),0,IF(ISNUMBER(E18),E18,N18)) + IF(ISBLANK(F18),0,IF(ISNUMBER(F18),F18,O18)) &gt; K18, NA(), IF(ISBLANK(B18),0,IF(ISNUMBER(B18),B18,K18)) + IF(ISBLANK(C18),0,IF(ISNUMBER(C18),C18,L18)) + IF(ISBLANK(D18),0,IF(ISNUMBER(D18),D18,M18)) + IF(ISBLANK(E18),0,IF(ISNUMBER(E18),E18,N18)) + IF(ISBLANK(F18),0,IF(ISNUMBER(F18),F18,O18))),NA())</f>
+        <v>4</v>
+      </c>
+      <c r="K18" s="12">
+        <v>5</v>
+      </c>
+      <c r="L18" s="12">
+        <v>4</v>
+      </c>
+      <c r="M18" s="12">
+        <v>3</v>
+      </c>
+      <c r="N18" s="12">
+        <v>2</v>
+      </c>
+      <c r="O18" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="3">
+        <f>SUM(G20:G22)/SUM(K20:K22) * K19</f>
         <v>12.5</v>
       </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="3">
-        <f>IF(ISBLANK(H18),G18,H18)</f>
+      <c r="H19" s="11"/>
+      <c r="I19" s="3">
+        <f>IF(ISBLANK(H19),G19,H19)</f>
         <v>12.5</v>
       </c>
-      <c r="K18">
+      <c r="K19">
         <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="12"/>
-      <c r="C19" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="13">
-        <f>IF(IF(ISBLANK(B19),0,1) + IF(ISBLANK(C19),0,1) + IF(ISBLANK(D19),0,1) + IF(ISBLANK(E19),0,1) + IF(ISBLANK(F19),0,1) = 1,IF(IF(ISBLANK(B19),0,IF(ISNUMBER(B19),B19,K19)) + IF(ISBLANK(C19),0,IF(ISNUMBER(C19),C19,L19)) + IF(ISBLANK(D19),0,IF(ISNUMBER(D19),D19,M19)) + IF(ISBLANK(E19),0,IF(ISNUMBER(E19),E19,N19)) + IF(ISBLANK(F19),0,IF(ISNUMBER(F19),F19,O19)) &gt; K19, NA(), IF(ISBLANK(B19),0,IF(ISNUMBER(B19),B19,K19)) + IF(ISBLANK(C19),0,IF(ISNUMBER(C19),C19,L19)) + IF(ISBLANK(D19),0,IF(ISNUMBER(D19),D19,M19)) + IF(ISBLANK(E19),0,IF(ISNUMBER(E19),E19,N19)) + IF(ISBLANK(F19),0,IF(ISNUMBER(F19),F19,O19))),NA())</f>
-        <v>4</v>
-      </c>
-      <c r="K19" s="12">
-        <v>5</v>
-      </c>
-      <c r="L19" s="12">
-        <v>4</v>
-      </c>
-      <c r="M19" s="12">
-        <v>3</v>
-      </c>
-      <c r="N19" s="12">
-        <v>2</v>
-      </c>
-      <c r="O19" s="12">
-        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="16" x14ac:dyDescent="0.2">
@@ -2518,7 +2546,7 @@
       </c>
       <c r="B20" s="12"/>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G20" s="13">
         <f>IF(IF(ISBLANK(B20),0,1) + IF(ISBLANK(C20),0,1) + IF(ISBLANK(D20),0,1) + IF(ISBLANK(E20),0,1) + IF(ISBLANK(F20),0,1) = 1,IF(IF(ISBLANK(B20),0,IF(ISNUMBER(B20),B20,K20)) + IF(ISBLANK(C20),0,IF(ISNUMBER(C20),C20,L20)) + IF(ISBLANK(D20),0,IF(ISNUMBER(D20),D20,M20)) + IF(ISBLANK(E20),0,IF(ISNUMBER(E20),E20,N20)) + IF(ISBLANK(F20),0,IF(ISNUMBER(F20),F20,O20)) &gt; K20, NA(), IF(ISBLANK(B20),0,IF(ISNUMBER(B20),B20,K20)) + IF(ISBLANK(C20),0,IF(ISNUMBER(C20),C20,L20)) + IF(ISBLANK(D20),0,IF(ISNUMBER(D20),D20,M20)) + IF(ISBLANK(E20),0,IF(ISNUMBER(E20),E20,N20)) + IF(ISBLANK(F20),0,IF(ISNUMBER(F20),F20,O20))),NA())</f>
@@ -2546,102 +2574,130 @@
       </c>
       <c r="B21" s="12"/>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G21" s="13">
         <f>IF(IF(ISBLANK(B21),0,1) + IF(ISBLANK(C21),0,1) + IF(ISBLANK(D21),0,1) + IF(ISBLANK(E21),0,1) + IF(ISBLANK(F21),0,1) = 1,IF(IF(ISBLANK(B21),0,IF(ISNUMBER(B21),B21,K21)) + IF(ISBLANK(C21),0,IF(ISNUMBER(C21),C21,L21)) + IF(ISBLANK(D21),0,IF(ISNUMBER(D21),D21,M21)) + IF(ISBLANK(E21),0,IF(ISNUMBER(E21),E21,N21)) + IF(ISBLANK(F21),0,IF(ISNUMBER(F21),F21,O21)) &gt; K21, NA(), IF(ISBLANK(B21),0,IF(ISNUMBER(B21),B21,K21)) + IF(ISBLANK(C21),0,IF(ISNUMBER(C21),C21,L21)) + IF(ISBLANK(D21),0,IF(ISNUMBER(D21),D21,M21)) + IF(ISBLANK(E21),0,IF(ISNUMBER(E21),E21,N21)) + IF(ISBLANK(F21),0,IF(ISNUMBER(F21),F21,O21))),NA())</f>
+        <v>4</v>
+      </c>
+      <c r="K21" s="12">
+        <v>5</v>
+      </c>
+      <c r="L21" s="12">
+        <v>4</v>
+      </c>
+      <c r="M21" s="12">
+        <v>3</v>
+      </c>
+      <c r="N21" s="12">
+        <v>2</v>
+      </c>
+      <c r="O21" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="13">
+        <f>IF(IF(ISBLANK(B22),0,1) + IF(ISBLANK(C22),0,1) + IF(ISBLANK(D22),0,1) + IF(ISBLANK(E22),0,1) + IF(ISBLANK(F22),0,1) = 1,IF(IF(ISBLANK(B22),0,IF(ISNUMBER(B22),B22,K22)) + IF(ISBLANK(C22),0,IF(ISNUMBER(C22),C22,L22)) + IF(ISBLANK(D22),0,IF(ISNUMBER(D22),D22,M22)) + IF(ISBLANK(E22),0,IF(ISNUMBER(E22),E22,N22)) + IF(ISBLANK(F22),0,IF(ISNUMBER(F22),F22,O22)) &gt; K22, NA(), IF(ISBLANK(B22),0,IF(ISNUMBER(B22),B22,K22)) + IF(ISBLANK(C22),0,IF(ISNUMBER(C22),C22,L22)) + IF(ISBLANK(D22),0,IF(ISNUMBER(D22),D22,M22)) + IF(ISBLANK(E22),0,IF(ISNUMBER(E22),E22,N22)) + IF(ISBLANK(F22),0,IF(ISNUMBER(F22),F22,O22))),NA())</f>
         <v>17</v>
       </c>
-      <c r="K21" s="12">
+      <c r="K22" s="12">
         <v>20</v>
       </c>
-      <c r="L21" s="12">
+      <c r="L22" s="12">
         <v>17</v>
       </c>
-      <c r="M21" s="12">
+      <c r="M22" s="12">
         <v>15</v>
       </c>
-      <c r="N21" s="12">
+      <c r="N22" s="12">
         <v>13</v>
       </c>
-      <c r="O21" s="12">
+      <c r="O22" s="12">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B10:B13">
-    <cfRule type="expression" dxfId="14" priority="1" stopIfTrue="1">
-      <formula>NOT(ISBLANK(B10))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15:B17">
-    <cfRule type="expression" dxfId="13" priority="21" stopIfTrue="1">
-      <formula>NOT(ISBLANK(B15))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19:B21">
-    <cfRule type="expression" dxfId="12" priority="36" stopIfTrue="1">
-      <formula>NOT(ISBLANK(B19))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10:C13">
-    <cfRule type="expression" dxfId="11" priority="2" stopIfTrue="1">
-      <formula>NOT(ISBLANK(C10))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15:C17">
-    <cfRule type="expression" dxfId="10" priority="22" stopIfTrue="1">
-      <formula>NOT(ISBLANK(C15))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19:C21">
-    <cfRule type="expression" dxfId="9" priority="37" stopIfTrue="1">
-      <formula>NOT(ISBLANK(C19))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D10:D13">
-    <cfRule type="expression" dxfId="8" priority="3" stopIfTrue="1">
-      <formula>NOT(ISBLANK(D10))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D15:D17">
-    <cfRule type="expression" dxfId="7" priority="23" stopIfTrue="1">
-      <formula>NOT(ISBLANK(D15))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D19:D21">
-    <cfRule type="expression" dxfId="6" priority="38" stopIfTrue="1">
-      <formula>NOT(ISBLANK(D19))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E10:E13">
-    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
-      <formula>NOT(ISBLANK(E10))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E15:E17">
-    <cfRule type="expression" dxfId="4" priority="24" stopIfTrue="1">
-      <formula>NOT(ISBLANK(E15))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E19:E21">
-    <cfRule type="expression" dxfId="3" priority="39" stopIfTrue="1">
-      <formula>NOT(ISBLANK(E19))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F10:F13">
-    <cfRule type="expression" dxfId="2" priority="5" stopIfTrue="1">
-      <formula>NOT(ISBLANK(F10))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F15:F17">
-    <cfRule type="expression" dxfId="1" priority="25" stopIfTrue="1">
-      <formula>NOT(ISBLANK(F15))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F19:F21">
-    <cfRule type="expression" dxfId="0" priority="40" stopIfTrue="1">
-      <formula>NOT(ISBLANK(F19))</formula>
+  <conditionalFormatting sqref="B11:B14">
+    <cfRule type="expression" dxfId="17" priority="4" stopIfTrue="1">
+      <formula>NOT(ISBLANK(B11))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16:B18">
+    <cfRule type="expression" dxfId="16" priority="24" stopIfTrue="1">
+      <formula>NOT(ISBLANK(B16))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20:B22">
+    <cfRule type="expression" dxfId="15" priority="39" stopIfTrue="1">
+      <formula>NOT(ISBLANK(B20))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11:D14">
+    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
+      <formula>NOT(ISBLANK(D11))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:D18">
+    <cfRule type="expression" dxfId="10" priority="26" stopIfTrue="1">
+      <formula>NOT(ISBLANK(D16))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20:D22">
+    <cfRule type="expression" dxfId="9" priority="41" stopIfTrue="1">
+      <formula>NOT(ISBLANK(D20))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11:E14">
+    <cfRule type="expression" dxfId="8" priority="7" stopIfTrue="1">
+      <formula>NOT(ISBLANK(E11))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16:E18">
+    <cfRule type="expression" dxfId="7" priority="27" stopIfTrue="1">
+      <formula>NOT(ISBLANK(E16))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20:E22">
+    <cfRule type="expression" dxfId="6" priority="42" stopIfTrue="1">
+      <formula>NOT(ISBLANK(E20))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11:F14">
+    <cfRule type="expression" dxfId="5" priority="8" stopIfTrue="1">
+      <formula>NOT(ISBLANK(F11))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16:F18">
+    <cfRule type="expression" dxfId="4" priority="28" stopIfTrue="1">
+      <formula>NOT(ISBLANK(F16))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20:F22">
+    <cfRule type="expression" dxfId="3" priority="43" stopIfTrue="1">
+      <formula>NOT(ISBLANK(F20))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:C14">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+      <formula>NOT(ISBLANK(C11))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16:C18">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+      <formula>NOT(ISBLANK(C16))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20:C22">
+    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
+      <formula>NOT(ISBLANK(C20))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Ajout de la note globale manuelle
</commit_message>
<xml_diff>
--- a/tests/fixtures/grille_gradebook.xlsx
+++ b/tests/fixtures/grille_gradebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Git repo - prof/c3hm/tests/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varch\Git-repos\c3hm\tests\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E9B006-3395-5E46-A9DB-382D0A5A97A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42FFEB19-FE98-4368-8E30-D680E36E293C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1583" yWindow="660" windowWidth="26100" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="houle" sheetId="1" r:id="rId1"/>
@@ -18,90 +18,93 @@
     <sheet name="gc_rhum" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="cthm_C2_comment" localSheetId="1">archibord!$J$16</definedName>
-    <definedName name="cthm_C2_comment" localSheetId="2">gc_rhum!$J$16</definedName>
-    <definedName name="cthm_C2_comment" localSheetId="0">houle!$J$16</definedName>
-    <definedName name="cthm_C2_grade_overwrite" localSheetId="1">archibord!$H$16</definedName>
-    <definedName name="cthm_C2_grade_overwrite" localSheetId="2">gc_rhum!$H$16</definedName>
-    <definedName name="cthm_C2_grade_overwrite" localSheetId="0">houle!$H$16</definedName>
-    <definedName name="cthm_C2_I1_comment" localSheetId="1">archibord!$J$17</definedName>
-    <definedName name="cthm_C2_I1_comment" localSheetId="2">gc_rhum!$J$17</definedName>
-    <definedName name="cthm_C2_I1_comment" localSheetId="0">houle!$J$17</definedName>
-    <definedName name="cthm_C2_I1_grade" localSheetId="1">archibord!$G$17</definedName>
-    <definedName name="cthm_C2_I1_grade" localSheetId="2">gc_rhum!$G$17</definedName>
-    <definedName name="cthm_C2_I1_grade" localSheetId="0">houle!$G$17</definedName>
-    <definedName name="cthm_C2_I2_comment" localSheetId="1">archibord!$J$18</definedName>
-    <definedName name="cthm_C2_I2_comment" localSheetId="2">gc_rhum!$J$18</definedName>
-    <definedName name="cthm_C2_I2_comment" localSheetId="0">houle!$J$18</definedName>
-    <definedName name="cthm_C2_I2_grade" localSheetId="1">archibord!$G$18</definedName>
-    <definedName name="cthm_C2_I2_grade" localSheetId="2">gc_rhum!$G$18</definedName>
-    <definedName name="cthm_C2_I2_grade" localSheetId="0">houle!$G$18</definedName>
-    <definedName name="cthm_C2_I3_comment" localSheetId="1">archibord!$J$19</definedName>
-    <definedName name="cthm_C2_I3_comment" localSheetId="2">gc_rhum!$J$19</definedName>
-    <definedName name="cthm_C2_I3_comment" localSheetId="0">houle!$J$19</definedName>
-    <definedName name="cthm_C2_I3_grade" localSheetId="1">archibord!$G$19</definedName>
-    <definedName name="cthm_C2_I3_grade" localSheetId="2">gc_rhum!$G$19</definedName>
-    <definedName name="cthm_C2_I3_grade" localSheetId="0">houle!$G$19</definedName>
-    <definedName name="cthm_C3_comment" localSheetId="1">archibord!$J$20</definedName>
-    <definedName name="cthm_C3_comment" localSheetId="2">gc_rhum!$J$20</definedName>
-    <definedName name="cthm_C3_comment" localSheetId="0">houle!$J$20</definedName>
-    <definedName name="cthm_C3_grade_overwrite" localSheetId="1">archibord!$H$20</definedName>
-    <definedName name="cthm_C3_grade_overwrite" localSheetId="2">gc_rhum!$H$20</definedName>
-    <definedName name="cthm_C3_grade_overwrite" localSheetId="0">houle!$H$20</definedName>
-    <definedName name="cthm_C3_I1_comment" localSheetId="1">archibord!$J$21</definedName>
-    <definedName name="cthm_C3_I1_comment" localSheetId="2">gc_rhum!$J$21</definedName>
-    <definedName name="cthm_C3_I1_comment" localSheetId="0">houle!$J$21</definedName>
-    <definedName name="cthm_C3_I1_grade" localSheetId="1">archibord!$G$21</definedName>
-    <definedName name="cthm_C3_I1_grade" localSheetId="2">gc_rhum!$G$21</definedName>
-    <definedName name="cthm_C3_I1_grade" localSheetId="0">houle!$G$21</definedName>
-    <definedName name="cthm_C3_I2_comment" localSheetId="1">archibord!$J$22</definedName>
-    <definedName name="cthm_C3_I2_comment" localSheetId="2">gc_rhum!$J$22</definedName>
-    <definedName name="cthm_C3_I2_comment" localSheetId="0">houle!$J$22</definedName>
-    <definedName name="cthm_C3_I2_grade" localSheetId="1">archibord!$G$22</definedName>
-    <definedName name="cthm_C3_I2_grade" localSheetId="2">gc_rhum!$G$22</definedName>
-    <definedName name="cthm_C3_I2_grade" localSheetId="0">houle!$G$22</definedName>
-    <definedName name="cthm_C3_I3_comment" localSheetId="1">archibord!$J$23</definedName>
-    <definedName name="cthm_C3_I3_comment" localSheetId="2">gc_rhum!$J$23</definedName>
-    <definedName name="cthm_C3_I3_comment" localSheetId="0">houle!$J$23</definedName>
-    <definedName name="cthm_C3_I3_grade" localSheetId="1">archibord!$G$23</definedName>
-    <definedName name="cthm_C3_I3_grade" localSheetId="2">gc_rhum!$G$23</definedName>
-    <definedName name="cthm_C3_I3_grade" localSheetId="0">houle!$G$23</definedName>
+    <definedName name="cthm_C2_comment" localSheetId="1">archibord!$J$17</definedName>
+    <definedName name="cthm_C2_comment" localSheetId="2">gc_rhum!$J$17</definedName>
+    <definedName name="cthm_C2_comment" localSheetId="0">houle!$J$17</definedName>
+    <definedName name="cthm_C2_grade_overwrite" localSheetId="1">archibord!$H$17</definedName>
+    <definedName name="cthm_C2_grade_overwrite" localSheetId="2">gc_rhum!$H$17</definedName>
+    <definedName name="cthm_C2_grade_overwrite" localSheetId="0">houle!$H$17</definedName>
+    <definedName name="cthm_C2_I1_comment" localSheetId="1">archibord!$J$18</definedName>
+    <definedName name="cthm_C2_I1_comment" localSheetId="2">gc_rhum!$J$18</definedName>
+    <definedName name="cthm_C2_I1_comment" localSheetId="0">houle!$J$18</definedName>
+    <definedName name="cthm_C2_I1_grade" localSheetId="1">archibord!$G$18</definedName>
+    <definedName name="cthm_C2_I1_grade" localSheetId="2">gc_rhum!$G$18</definedName>
+    <definedName name="cthm_C2_I1_grade" localSheetId="0">houle!$G$18</definedName>
+    <definedName name="cthm_C2_I2_comment" localSheetId="1">archibord!$J$19</definedName>
+    <definedName name="cthm_C2_I2_comment" localSheetId="2">gc_rhum!$J$19</definedName>
+    <definedName name="cthm_C2_I2_comment" localSheetId="0">houle!$J$19</definedName>
+    <definedName name="cthm_C2_I2_grade" localSheetId="1">archibord!$G$19</definedName>
+    <definedName name="cthm_C2_I2_grade" localSheetId="2">gc_rhum!$G$19</definedName>
+    <definedName name="cthm_C2_I2_grade" localSheetId="0">houle!$G$19</definedName>
+    <definedName name="cthm_C2_I3_comment" localSheetId="1">archibord!$J$20</definedName>
+    <definedName name="cthm_C2_I3_comment" localSheetId="2">gc_rhum!$J$20</definedName>
+    <definedName name="cthm_C2_I3_comment" localSheetId="0">houle!$J$20</definedName>
+    <definedName name="cthm_C2_I3_grade" localSheetId="1">archibord!$G$20</definedName>
+    <definedName name="cthm_C2_I3_grade" localSheetId="2">gc_rhum!$G$20</definedName>
+    <definedName name="cthm_C2_I3_grade" localSheetId="0">houle!$G$20</definedName>
+    <definedName name="cthm_C3_comment" localSheetId="1">archibord!$J$21</definedName>
+    <definedName name="cthm_C3_comment" localSheetId="2">gc_rhum!$J$21</definedName>
+    <definedName name="cthm_C3_comment" localSheetId="0">houle!$J$21</definedName>
+    <definedName name="cthm_C3_grade_overwrite" localSheetId="1">archibord!$H$21</definedName>
+    <definedName name="cthm_C3_grade_overwrite" localSheetId="2">gc_rhum!$H$21</definedName>
+    <definedName name="cthm_C3_grade_overwrite" localSheetId="0">houle!$H$21</definedName>
+    <definedName name="cthm_C3_I1_comment" localSheetId="1">archibord!$J$22</definedName>
+    <definedName name="cthm_C3_I1_comment" localSheetId="2">gc_rhum!$J$22</definedName>
+    <definedName name="cthm_C3_I1_comment" localSheetId="0">houle!$J$22</definedName>
+    <definedName name="cthm_C3_I1_grade" localSheetId="1">archibord!$G$22</definedName>
+    <definedName name="cthm_C3_I1_grade" localSheetId="2">gc_rhum!$G$22</definedName>
+    <definedName name="cthm_C3_I1_grade" localSheetId="0">houle!$G$22</definedName>
+    <definedName name="cthm_C3_I2_comment" localSheetId="1">archibord!$J$23</definedName>
+    <definedName name="cthm_C3_I2_comment" localSheetId="2">gc_rhum!$J$23</definedName>
+    <definedName name="cthm_C3_I2_comment" localSheetId="0">houle!$J$23</definedName>
+    <definedName name="cthm_C3_I2_grade" localSheetId="1">archibord!$G$23</definedName>
+    <definedName name="cthm_C3_I2_grade" localSheetId="2">gc_rhum!$G$23</definedName>
+    <definedName name="cthm_C3_I2_grade" localSheetId="0">houle!$G$23</definedName>
+    <definedName name="cthm_C3_I3_comment" localSheetId="1">archibord!$J$24</definedName>
+    <definedName name="cthm_C3_I3_comment" localSheetId="2">gc_rhum!$J$24</definedName>
+    <definedName name="cthm_C3_I3_comment" localSheetId="0">houle!$J$24</definedName>
+    <definedName name="cthm_C3_I3_grade" localSheetId="1">archibord!$G$24</definedName>
+    <definedName name="cthm_C3_I3_grade" localSheetId="2">gc_rhum!$G$24</definedName>
+    <definedName name="cthm_C3_I3_grade" localSheetId="0">houle!$G$24</definedName>
     <definedName name="cthm_global_comment" localSheetId="1">archibord!$B$5</definedName>
     <definedName name="cthm_global_comment" localSheetId="2">gc_rhum!$B$5</definedName>
     <definedName name="cthm_global_comment" localSheetId="0">houle!$B$5</definedName>
+    <definedName name="cthm_global_grade" localSheetId="1">archibord!$C$8</definedName>
+    <definedName name="cthm_global_grade" localSheetId="2">gc_rhum!$C$8</definedName>
+    <definedName name="cthm_global_grade" localSheetId="0">houle!$C$8</definedName>
     <definedName name="cthm_omnivox" localSheetId="1">archibord!$B$4</definedName>
     <definedName name="cthm_omnivox" localSheetId="2">gc_rhum!$B$4</definedName>
     <definedName name="cthm_omnivox" localSheetId="0">houle!$B$4</definedName>
-    <definedName name="lessivage_balai_comment" localSheetId="1">archibord!$J$12</definedName>
-    <definedName name="lessivage_balai_comment" localSheetId="2">gc_rhum!$J$12</definedName>
-    <definedName name="lessivage_balai_comment" localSheetId="0">houle!$J$12</definedName>
-    <definedName name="lessivage_balai_grade" localSheetId="1">archibord!$G$12</definedName>
-    <definedName name="lessivage_balai_grade" localSheetId="2">gc_rhum!$G$12</definedName>
-    <definedName name="lessivage_balai_grade" localSheetId="0">houle!$G$12</definedName>
-    <definedName name="lessivage_comment" localSheetId="1">archibord!$J$11</definedName>
-    <definedName name="lessivage_comment" localSheetId="2">gc_rhum!$J$11</definedName>
-    <definedName name="lessivage_comment" localSheetId="0">houle!$J$11</definedName>
-    <definedName name="lessivage_grade_overwrite" localSheetId="1">archibord!$H$11</definedName>
-    <definedName name="lessivage_grade_overwrite" localSheetId="2">gc_rhum!$H$11</definedName>
-    <definedName name="lessivage_grade_overwrite" localSheetId="0">houle!$H$11</definedName>
-    <definedName name="lessivage_I2_comment" localSheetId="1">archibord!$J$13</definedName>
-    <definedName name="lessivage_I2_comment" localSheetId="2">gc_rhum!$J$13</definedName>
-    <definedName name="lessivage_I2_comment" localSheetId="0">houle!$J$13</definedName>
-    <definedName name="lessivage_I2_grade" localSheetId="1">archibord!$G$13</definedName>
-    <definedName name="lessivage_I2_grade" localSheetId="2">gc_rhum!$G$13</definedName>
-    <definedName name="lessivage_I2_grade" localSheetId="0">houle!$G$13</definedName>
-    <definedName name="lessivage_I3_comment" localSheetId="1">archibord!$J$14</definedName>
-    <definedName name="lessivage_I3_comment" localSheetId="2">gc_rhum!$J$14</definedName>
-    <definedName name="lessivage_I3_comment" localSheetId="0">houle!$J$14</definedName>
-    <definedName name="lessivage_I3_grade" localSheetId="1">archibord!$G$14</definedName>
-    <definedName name="lessivage_I3_grade" localSheetId="2">gc_rhum!$G$14</definedName>
-    <definedName name="lessivage_I3_grade" localSheetId="0">houle!$G$14</definedName>
-    <definedName name="lessivage_I4_comment" localSheetId="1">archibord!$J$15</definedName>
-    <definedName name="lessivage_I4_comment" localSheetId="2">gc_rhum!$J$15</definedName>
-    <definedName name="lessivage_I4_comment" localSheetId="0">houle!$J$15</definedName>
-    <definedName name="lessivage_I4_grade" localSheetId="1">archibord!$G$15</definedName>
-    <definedName name="lessivage_I4_grade" localSheetId="2">gc_rhum!$G$15</definedName>
-    <definedName name="lessivage_I4_grade" localSheetId="0">houle!$G$15</definedName>
+    <definedName name="lessivage_balai_comment" localSheetId="1">archibord!$J$13</definedName>
+    <definedName name="lessivage_balai_comment" localSheetId="2">gc_rhum!$J$13</definedName>
+    <definedName name="lessivage_balai_comment" localSheetId="0">houle!$J$13</definedName>
+    <definedName name="lessivage_balai_grade" localSheetId="1">archibord!$G$13</definedName>
+    <definedName name="lessivage_balai_grade" localSheetId="2">gc_rhum!$G$13</definedName>
+    <definedName name="lessivage_balai_grade" localSheetId="0">houle!$G$13</definedName>
+    <definedName name="lessivage_comment" localSheetId="1">archibord!$J$12</definedName>
+    <definedName name="lessivage_comment" localSheetId="2">gc_rhum!$J$12</definedName>
+    <definedName name="lessivage_comment" localSheetId="0">houle!$J$12</definedName>
+    <definedName name="lessivage_grade_overwrite" localSheetId="1">archibord!$H$12</definedName>
+    <definedName name="lessivage_grade_overwrite" localSheetId="2">gc_rhum!$H$12</definedName>
+    <definedName name="lessivage_grade_overwrite" localSheetId="0">houle!$H$12</definedName>
+    <definedName name="lessivage_I2_comment" localSheetId="1">archibord!$J$14</definedName>
+    <definedName name="lessivage_I2_comment" localSheetId="2">gc_rhum!$J$14</definedName>
+    <definedName name="lessivage_I2_comment" localSheetId="0">houle!$J$14</definedName>
+    <definedName name="lessivage_I2_grade" localSheetId="1">archibord!$G$14</definedName>
+    <definedName name="lessivage_I2_grade" localSheetId="2">gc_rhum!$G$14</definedName>
+    <definedName name="lessivage_I2_grade" localSheetId="0">houle!$G$14</definedName>
+    <definedName name="lessivage_I3_comment" localSheetId="1">archibord!$J$15</definedName>
+    <definedName name="lessivage_I3_comment" localSheetId="2">gc_rhum!$J$15</definedName>
+    <definedName name="lessivage_I3_comment" localSheetId="0">houle!$J$15</definedName>
+    <definedName name="lessivage_I3_grade" localSheetId="1">archibord!$G$15</definedName>
+    <definedName name="lessivage_I3_grade" localSheetId="2">gc_rhum!$G$15</definedName>
+    <definedName name="lessivage_I3_grade" localSheetId="0">houle!$G$15</definedName>
+    <definedName name="lessivage_I4_comment" localSheetId="1">archibord!$J$16</definedName>
+    <definedName name="lessivage_I4_comment" localSheetId="2">gc_rhum!$J$16</definedName>
+    <definedName name="lessivage_I4_comment" localSheetId="0">houle!$J$16</definedName>
+    <definedName name="lessivage_I4_grade" localSheetId="1">archibord!$G$16</definedName>
+    <definedName name="lessivage_I4_grade" localSheetId="2">gc_rhum!$G$16</definedName>
+    <definedName name="lessivage_I4_grade" localSheetId="0">houle!$G$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -121,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="58">
   <si>
     <t>Grille d'évaluation – 420-C3HM-MA – Le Grand Carénage des Flibustiers</t>
   </si>
@@ -141,6 +144,12 @@
     <t>Commentaire général</t>
   </si>
   <si>
+    <t>note calculée</t>
+  </si>
+  <si>
+    <t>note manuelle</t>
+  </si>
+  <si>
     <t>Total sur 100</t>
   </si>
   <si>
@@ -174,12 +183,6 @@
     <t>Insuffisant</t>
   </si>
   <si>
-    <t>note calculée</t>
-  </si>
-  <si>
-    <t>note manuelle</t>
-  </si>
-  <si>
     <t>note</t>
   </si>
   <si>
@@ -240,16 +243,19 @@
     <t>x</t>
   </si>
   <si>
+    <t>Commentaire critère 1</t>
+  </si>
+  <si>
+    <t>Commentaire critère 2</t>
+  </si>
+  <si>
+    <t>Commentaire critère 3</t>
+  </si>
+  <si>
     <t>Super bon travail !</t>
   </si>
   <si>
-    <t>Commentaire critère 1</t>
-  </si>
-  <si>
-    <t>Commentaire critère 2</t>
-  </si>
-  <si>
-    <t>Commentaire critère 3</t>
+    <t>Vous allez être jeté par-dessus bord !</t>
   </si>
   <si>
     <t>A</t>
@@ -289,9 +295,6 @@
   </si>
   <si>
     <t>M</t>
-  </si>
-  <si>
-    <t>Vous allez être jeté par-dessus bord !</t>
   </si>
   <si>
     <t>Bravo !</t>
@@ -322,6 +325,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -337,24 +348,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="12"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <i/>
       <sz val="12"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -378,6 +381,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
     <fill>
@@ -408,11 +416,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC8C8"/>
         <bgColor rgb="FFFFC8C8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
@@ -476,42 +479,187 @@
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="5" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="5" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="5" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="5" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="5" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="6"/>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="2" xfId="7" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="5"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="7"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="5" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="8" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Calcul" xfId="3" builtinId="22"/>
-    <cellStyle name="Entrée" xfId="7" builtinId="20"/>
+    <cellStyle name="Calculation" xfId="4" builtinId="22"/>
+    <cellStyle name="Explanatory Text" xfId="6" builtinId="53"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="7" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="2" builtinId="19"/>
+    <cellStyle name="Input" xfId="5" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Sortie" xfId="8" builtinId="21"/>
-    <cellStyle name="Texte explicatif" xfId="4" builtinId="53"/>
-    <cellStyle name="Titre" xfId="1" builtinId="15"/>
-    <cellStyle name="Titre 2" xfId="2" builtinId="17"/>
-    <cellStyle name="Titre 3" xfId="6" builtinId="18"/>
-    <cellStyle name="Titre 4" xfId="5" builtinId="19"/>
+    <cellStyle name="Output" xfId="8" builtinId="21"/>
+    <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="63">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF0FFB0"/>
+          <bgColor rgb="FFF0FFB0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF0FFB0"/>
+          <bgColor rgb="FFF0FFB0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF0FFB0"/>
+          <bgColor rgb="FFF0FFB0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC8C8"/>
+          <bgColor rgb="FFFFC8C8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC8C8"/>
+          <bgColor rgb="FFFFC8C8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC8C8"/>
+          <bgColor rgb="FFFFC8C8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE4C8"/>
+          <bgColor rgb="FFFFE4C8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE4C8"/>
+          <bgColor rgb="FFFFE4C8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE4C8"/>
+          <bgColor rgb="FFFFE4C8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF8C2"/>
+          <bgColor rgb="FFFFF8C2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF8C2"/>
+          <bgColor rgb="FFFFF8C2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF8C2"/>
+          <bgColor rgb="FFFFF8C2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF0FFB0"/>
+          <bgColor rgb="FFF0FFB0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF0FFB0"/>
+          <bgColor rgb="FFF0FFB0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF0FFB0"/>
+          <bgColor rgb="FFF0FFB0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC8FFC8"/>
+          <bgColor rgb="FFC8FFC8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC8FFC8"/>
+          <bgColor rgb="FFC8FFC8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC8FFC8"/>
+          <bgColor rgb="FFC8FFC8"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1170,13 +1318,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="50" customWidth="1"/>
     <col min="2" max="9" width="15" customWidth="1"/>
@@ -1184,12 +1332,12 @@
     <col min="11" max="15" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="22.5" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1197,7 +1345,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1205,314 +1353,323 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="16.899999999999999" x14ac:dyDescent="0.5">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4">
+        <f>IF(ISBLANK(C8),SUM(I12*30,I17*40,I21*30)/100, C8)</f>
+        <v>96.4</v>
+      </c>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A12" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="4">
+        <f>(10 * G13 + 10 * G14 + 5 * G15 + 5 * G16) / 30</f>
+        <v>100</v>
+      </c>
+      <c r="H12" s="13"/>
+      <c r="I12" s="4">
+        <f>IF(ISBLANK(H12),G12,H12)</f>
+        <v>100</v>
+      </c>
+      <c r="J12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3">
-        <f>SUM(I11*30,I16*40,I20*30)/100</f>
-        <v>96.4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="3">
-        <f>(10 * G12 + 10 * G13 + 5 * G14 + 5 * G15) / 30</f>
-        <v>100</v>
-      </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="3">
-        <f>IF(ISBLANK(H11),G11,H11)</f>
-        <v>100</v>
-      </c>
-      <c r="J11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="13">
-        <f>IF(IF(ISBLANK(B12),0,1) + IF(ISBLANK(C12),0,1) + IF(ISBLANK(D12),0,1) + IF(ISBLANK(E12),0,1) + IF(ISBLANK(F12),0,1) = 1,IF(IF(ISBLANK(B12),0,IF(ISNUMBER(B12),B12,100)) + IF(ISBLANK(C12),0,IF(ISNUMBER(C12),C12,85)) + IF(ISBLANK(D12),0,IF(ISNUMBER(D12),D12,70)) + IF(ISBLANK(E12),0,IF(ISNUMBER(E12),E12,60)) + IF(ISBLANK(F12),0,IF(ISNUMBER(F12),F12,30)) &gt; 100, NA(), IF(ISBLANK(B12),0,IF(ISNUMBER(B12),B12,100)) + IF(ISBLANK(C12),0,IF(ISNUMBER(C12),C12,85)) + IF(ISBLANK(D12),0,IF(ISNUMBER(D12),D12,70)) + IF(ISBLANK(E12),0,IF(ISNUMBER(E12),E12,60)) + IF(ISBLANK(F12),0,IF(ISNUMBER(F12),F12,30))),NA())</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="B13" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="14">
         <f>IF(IF(ISBLANK(B13),0,1) + IF(ISBLANK(C13),0,1) + IF(ISBLANK(D13),0,1) + IF(ISBLANK(E13),0,1) + IF(ISBLANK(F13),0,1) = 1,IF(IF(ISBLANK(B13),0,IF(ISNUMBER(B13),B13,100)) + IF(ISBLANK(C13),0,IF(ISNUMBER(C13),C13,85)) + IF(ISBLANK(D13),0,IF(ISNUMBER(D13),D13,70)) + IF(ISBLANK(E13),0,IF(ISNUMBER(E13),E13,60)) + IF(ISBLANK(F13),0,IF(ISNUMBER(F13),F13,30)) &gt; 100, NA(), IF(ISBLANK(B13),0,IF(ISNUMBER(B13),B13,100)) + IF(ISBLANK(C13),0,IF(ISNUMBER(C13),C13,85)) + IF(ISBLANK(D13),0,IF(ISNUMBER(D13),D13,70)) + IF(ISBLANK(E13),0,IF(ISNUMBER(E13),E13,60)) + IF(ISBLANK(F13),0,IF(ISNUMBER(F13),F13,30))),NA())</f>
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>24</v>
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A14" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="B14" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="14">
         <f>IF(IF(ISBLANK(B14),0,1) + IF(ISBLANK(C14),0,1) + IF(ISBLANK(D14),0,1) + IF(ISBLANK(E14),0,1) + IF(ISBLANK(F14),0,1) = 1,IF(IF(ISBLANK(B14),0,IF(ISNUMBER(B14),B14,100)) + IF(ISBLANK(C14),0,IF(ISNUMBER(C14),C14,85)) + IF(ISBLANK(D14),0,IF(ISNUMBER(D14),D14,70)) + IF(ISBLANK(E14),0,IF(ISNUMBER(E14),E14,60)) + IF(ISBLANK(F14),0,IF(ISNUMBER(F14),F14,30)) &gt; 100, NA(), IF(ISBLANK(B14),0,IF(ISNUMBER(B14),B14,100)) + IF(ISBLANK(C14),0,IF(ISNUMBER(C14),C14,85)) + IF(ISBLANK(D14),0,IF(ISNUMBER(D14),D14,70)) + IF(ISBLANK(E14),0,IF(ISNUMBER(E14),E14,60)) + IF(ISBLANK(F14),0,IF(ISNUMBER(F14),F14,30))),NA())</f>
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>25</v>
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A15" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="B15" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="14">
         <f>IF(IF(ISBLANK(B15),0,1) + IF(ISBLANK(C15),0,1) + IF(ISBLANK(D15),0,1) + IF(ISBLANK(E15),0,1) + IF(ISBLANK(F15),0,1) = 1,IF(IF(ISBLANK(B15),0,IF(ISNUMBER(B15),B15,100)) + IF(ISBLANK(C15),0,IF(ISNUMBER(C15),C15,85)) + IF(ISBLANK(D15),0,IF(ISNUMBER(D15),D15,70)) + IF(ISBLANK(E15),0,IF(ISNUMBER(E15),E15,60)) + IF(ISBLANK(F15),0,IF(ISNUMBER(F15),F15,30)) &gt; 100, NA(), IF(ISBLANK(B15),0,IF(ISNUMBER(B15),B15,100)) + IF(ISBLANK(C15),0,IF(ISNUMBER(C15),C15,85)) + IF(ISBLANK(D15),0,IF(ISNUMBER(D15),D15,70)) + IF(ISBLANK(E15),0,IF(ISNUMBER(E15),E15,60)) + IF(ISBLANK(F15),0,IF(ISNUMBER(F15),F15,30))),NA())</f>
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="14">
+        <f>IF(IF(ISBLANK(B16),0,1) + IF(ISBLANK(C16),0,1) + IF(ISBLANK(D16),0,1) + IF(ISBLANK(E16),0,1) + IF(ISBLANK(F16),0,1) = 1,IF(IF(ISBLANK(B16),0,IF(ISNUMBER(B16),B16,100)) + IF(ISBLANK(C16),0,IF(ISNUMBER(C16),C16,85)) + IF(ISBLANK(D16),0,IF(ISNUMBER(D16),D16,70)) + IF(ISBLANK(E16),0,IF(ISNUMBER(E16),E16,60)) + IF(ISBLANK(F16),0,IF(ISNUMBER(F16),F16,30)) &gt; 100, NA(), IF(ISBLANK(B16),0,IF(ISNUMBER(B16),B16,100)) + IF(ISBLANK(C16),0,IF(ISNUMBER(C16),C16,85)) + IF(ISBLANK(D16),0,IF(ISNUMBER(D16),D16,70)) + IF(ISBLANK(E16),0,IF(ISNUMBER(E16),E16,60)) + IF(ISBLANK(F16),0,IF(ISNUMBER(F16),F16,30))),NA())</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A17" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="3">
-        <f>(14 * G17 + 13 * G18 + 13 * G19) / 40</f>
+      <c r="G17" s="4">
+        <f>(14 * G18 + 13 * G19 + 13 * G20) / 40</f>
         <v>94.75</v>
       </c>
-      <c r="H16" s="12"/>
-      <c r="I16" s="3">
-        <f>IF(ISBLANK(H16),G16,H16)</f>
+      <c r="H17" s="13"/>
+      <c r="I17" s="4">
+        <f>IF(ISBLANK(H17),G17,H17)</f>
         <v>94.75</v>
       </c>
-      <c r="J16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="J17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C17" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="13">
-        <f>IF(IF(ISBLANK(B17),0,1) + IF(ISBLANK(C17),0,1) + IF(ISBLANK(D17),0,1) + IF(ISBLANK(E17),0,1) + IF(ISBLANK(F17),0,1) = 1,IF(IF(ISBLANK(B17),0,IF(ISNUMBER(B17),B17,100)) + IF(ISBLANK(C17),0,IF(ISNUMBER(C17),C17,85)) + IF(ISBLANK(D17),0,IF(ISNUMBER(D17),D17,70)) + IF(ISBLANK(E17),0,IF(ISNUMBER(E17),E17,60)) + IF(ISBLANK(F17),0,IF(ISNUMBER(F17),F17,30)) &gt; 100, NA(), IF(ISBLANK(B17),0,IF(ISNUMBER(B17),B17,100)) + IF(ISBLANK(C17),0,IF(ISNUMBER(C17),C17,85)) + IF(ISBLANK(D17),0,IF(ISNUMBER(D17),D17,70)) + IF(ISBLANK(E17),0,IF(ISNUMBER(E17),E17,60)) + IF(ISBLANK(F17),0,IF(ISNUMBER(F17),F17,30))),NA())</f>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="14">
+        <f>IF(IF(ISBLANK(B18),0,1) + IF(ISBLANK(C18),0,1) + IF(ISBLANK(D18),0,1) + IF(ISBLANK(E18),0,1) + IF(ISBLANK(F18),0,1) = 1,IF(IF(ISBLANK(B18),0,IF(ISNUMBER(B18),B18,100)) + IF(ISBLANK(C18),0,IF(ISNUMBER(C18),C18,85)) + IF(ISBLANK(D18),0,IF(ISNUMBER(D18),D18,70)) + IF(ISBLANK(E18),0,IF(ISNUMBER(E18),E18,60)) + IF(ISBLANK(F18),0,IF(ISNUMBER(F18),F18,30)) &gt; 100, NA(), IF(ISBLANK(B18),0,IF(ISNUMBER(B18),B18,100)) + IF(ISBLANK(C18),0,IF(ISNUMBER(C18),C18,85)) + IF(ISBLANK(D18),0,IF(ISNUMBER(D18),D18,70)) + IF(ISBLANK(E18),0,IF(ISNUMBER(E18),E18,60)) + IF(ISBLANK(F18),0,IF(ISNUMBER(F18),F18,30))),NA())</f>
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A19" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="13">
-        <f>IF(IF(ISBLANK(B18),0,1) + IF(ISBLANK(C18),0,1) + IF(ISBLANK(D18),0,1) + IF(ISBLANK(E18),0,1) + IF(ISBLANK(F18),0,1) = 1,IF(IF(ISBLANK(B18),0,IF(ISNUMBER(B18),B18,100)) + IF(ISBLANK(C18),0,IF(ISNUMBER(C18),C18,85)) + IF(ISBLANK(D18),0,IF(ISNUMBER(D18),D18,70)) + IF(ISBLANK(E18),0,IF(ISNUMBER(E18),E18,60)) + IF(ISBLANK(F18),0,IF(ISNUMBER(F18),F18,30)) &gt; 100, NA(), IF(ISBLANK(B18),0,IF(ISNUMBER(B18),B18,100)) + IF(ISBLANK(C18),0,IF(ISNUMBER(C18),C18,85)) + IF(ISBLANK(D18),0,IF(ISNUMBER(D18),D18,70)) + IF(ISBLANK(E18),0,IF(ISNUMBER(E18),E18,60)) + IF(ISBLANK(F18),0,IF(ISNUMBER(F18),F18,30))),NA())</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="B19" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="14">
         <f>IF(IF(ISBLANK(B19),0,1) + IF(ISBLANK(C19),0,1) + IF(ISBLANK(D19),0,1) + IF(ISBLANK(E19),0,1) + IF(ISBLANK(F19),0,1) = 1,IF(IF(ISBLANK(B19),0,IF(ISNUMBER(B19),B19,100)) + IF(ISBLANK(C19),0,IF(ISNUMBER(C19),C19,85)) + IF(ISBLANK(D19),0,IF(ISNUMBER(D19),D19,70)) + IF(ISBLANK(E19),0,IF(ISNUMBER(E19),E19,60)) + IF(ISBLANK(F19),0,IF(ISNUMBER(F19),F19,30)) &gt; 100, NA(), IF(ISBLANK(B19),0,IF(ISNUMBER(B19),B19,100)) + IF(ISBLANK(C19),0,IF(ISNUMBER(C19),C19,85)) + IF(ISBLANK(D19),0,IF(ISNUMBER(D19),D19,70)) + IF(ISBLANK(E19),0,IF(ISNUMBER(E19),E19,60)) + IF(ISBLANK(F19),0,IF(ISNUMBER(F19),F19,30))),NA())</f>
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
+    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="14">
+        <f>IF(IF(ISBLANK(B20),0,1) + IF(ISBLANK(C20),0,1) + IF(ISBLANK(D20),0,1) + IF(ISBLANK(E20),0,1) + IF(ISBLANK(F20),0,1) = 1,IF(IF(ISBLANK(B20),0,IF(ISNUMBER(B20),B20,100)) + IF(ISBLANK(C20),0,IF(ISNUMBER(C20),C20,85)) + IF(ISBLANK(D20),0,IF(ISNUMBER(D20),D20,70)) + IF(ISBLANK(E20),0,IF(ISNUMBER(E20),E20,60)) + IF(ISBLANK(F20),0,IF(ISNUMBER(F20),F20,30)) &gt; 100, NA(), IF(ISBLANK(B20),0,IF(ISNUMBER(B20),B20,100)) + IF(ISBLANK(C20),0,IF(ISNUMBER(C20),C20,85)) + IF(ISBLANK(D20),0,IF(ISNUMBER(D20),D20,70)) + IF(ISBLANK(E20),0,IF(ISNUMBER(E20),E20,60)) + IF(ISBLANK(F20),0,IF(ISNUMBER(F20),F20,30))),NA())</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A21" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="3">
-        <f>(10 * G21 + 10 * G22 + 10 * G23) / 30</f>
+      <c r="G21" s="4">
+        <f>(10 * G22 + 10 * G23 + 10 * G24) / 30</f>
         <v>95</v>
       </c>
-      <c r="H20" s="12"/>
-      <c r="I20" s="3">
-        <f>IF(ISBLANK(H20),G20,H20)</f>
+      <c r="H21" s="13"/>
+      <c r="I21" s="4">
+        <f>IF(ISBLANK(H21),G21,H21)</f>
         <v>95</v>
       </c>
-      <c r="J20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="J21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A22" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B21" t="s">
-        <v>38</v>
-      </c>
-      <c r="G21" s="13">
-        <f>IF(IF(ISBLANK(B21),0,1) + IF(ISBLANK(C21),0,1) + IF(ISBLANK(D21),0,1) + IF(ISBLANK(E21),0,1) + IF(ISBLANK(F21),0,1) = 1,IF(IF(ISBLANK(B21),0,IF(ISNUMBER(B21),B21,100)) + IF(ISBLANK(C21),0,IF(ISNUMBER(C21),C21,85)) + IF(ISBLANK(D21),0,IF(ISNUMBER(D21),D21,70)) + IF(ISBLANK(E21),0,IF(ISNUMBER(E21),E21,60)) + IF(ISBLANK(F21),0,IF(ISNUMBER(F21),F21,30)) &gt; 100, NA(), IF(ISBLANK(B21),0,IF(ISNUMBER(B21),B21,100)) + IF(ISBLANK(C21),0,IF(ISNUMBER(C21),C21,85)) + IF(ISBLANK(D21),0,IF(ISNUMBER(D21),D21,70)) + IF(ISBLANK(E21),0,IF(ISNUMBER(E21),E21,60)) + IF(ISBLANK(F21),0,IF(ISNUMBER(F21),F21,30))),NA())</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="B22" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="14">
         <f>IF(IF(ISBLANK(B22),0,1) + IF(ISBLANK(C22),0,1) + IF(ISBLANK(D22),0,1) + IF(ISBLANK(E22),0,1) + IF(ISBLANK(F22),0,1) = 1,IF(IF(ISBLANK(B22),0,IF(ISNUMBER(B22),B22,100)) + IF(ISBLANK(C22),0,IF(ISNUMBER(C22),C22,85)) + IF(ISBLANK(D22),0,IF(ISNUMBER(D22),D22,70)) + IF(ISBLANK(E22),0,IF(ISNUMBER(E22),E22,60)) + IF(ISBLANK(F22),0,IF(ISNUMBER(F22),F22,30)) &gt; 100, NA(), IF(ISBLANK(B22),0,IF(ISNUMBER(B22),B22,100)) + IF(ISBLANK(C22),0,IF(ISNUMBER(C22),C22,85)) + IF(ISBLANK(D22),0,IF(ISNUMBER(D22),D22,70)) + IF(ISBLANK(E22),0,IF(ISNUMBER(E22),E22,60)) + IF(ISBLANK(F22),0,IF(ISNUMBER(F22),F22,30))),NA())</f>
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A23" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="14">
+        <f>IF(IF(ISBLANK(B23),0,1) + IF(ISBLANK(C23),0,1) + IF(ISBLANK(D23),0,1) + IF(ISBLANK(E23),0,1) + IF(ISBLANK(F23),0,1) = 1,IF(IF(ISBLANK(B23),0,IF(ISNUMBER(B23),B23,100)) + IF(ISBLANK(C23),0,IF(ISNUMBER(C23),C23,85)) + IF(ISBLANK(D23),0,IF(ISNUMBER(D23),D23,70)) + IF(ISBLANK(E23),0,IF(ISNUMBER(E23),E23,60)) + IF(ISBLANK(F23),0,IF(ISNUMBER(F23),F23,30)) &gt; 100, NA(), IF(ISBLANK(B23),0,IF(ISNUMBER(B23),B23,100)) + IF(ISBLANK(C23),0,IF(ISNUMBER(C23),C23,85)) + IF(ISBLANK(D23),0,IF(ISNUMBER(D23),D23,70)) + IF(ISBLANK(E23),0,IF(ISNUMBER(E23),E23,60)) + IF(ISBLANK(F23),0,IF(ISNUMBER(F23),F23,30))),NA())</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A24" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C23" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" s="13">
-        <f>IF(IF(ISBLANK(B23),0,1) + IF(ISBLANK(C23),0,1) + IF(ISBLANK(D23),0,1) + IF(ISBLANK(E23),0,1) + IF(ISBLANK(F23),0,1) = 1,IF(IF(ISBLANK(B23),0,IF(ISNUMBER(B23),B23,100)) + IF(ISBLANK(C23),0,IF(ISNUMBER(C23),C23,85)) + IF(ISBLANK(D23),0,IF(ISNUMBER(D23),D23,70)) + IF(ISBLANK(E23),0,IF(ISNUMBER(E23),E23,60)) + IF(ISBLANK(F23),0,IF(ISNUMBER(F23),F23,30)) &gt; 100, NA(), IF(ISBLANK(B23),0,IF(ISNUMBER(B23),B23,100)) + IF(ISBLANK(C23),0,IF(ISNUMBER(C23),C23,85)) + IF(ISBLANK(D23),0,IF(ISNUMBER(D23),D23,70)) + IF(ISBLANK(E23),0,IF(ISNUMBER(E23),E23,60)) + IF(ISBLANK(F23),0,IF(ISNUMBER(F23),F23,30))),NA())</f>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="14">
+        <f>IF(IF(ISBLANK(B24),0,1) + IF(ISBLANK(C24),0,1) + IF(ISBLANK(D24),0,1) + IF(ISBLANK(E24),0,1) + IF(ISBLANK(F24),0,1) = 1,IF(IF(ISBLANK(B24),0,IF(ISNUMBER(B24),B24,100)) + IF(ISBLANK(C24),0,IF(ISNUMBER(C24),C24,85)) + IF(ISBLANK(D24),0,IF(ISNUMBER(D24),D24,70)) + IF(ISBLANK(E24),0,IF(ISNUMBER(E24),E24,60)) + IF(ISBLANK(F24),0,IF(ISNUMBER(F24),F24,30)) &gt; 100, NA(), IF(ISBLANK(B24),0,IF(ISNUMBER(B24),B24,100)) + IF(ISBLANK(C24),0,IF(ISNUMBER(C24),C24,85)) + IF(ISBLANK(D24),0,IF(ISNUMBER(D24),D24,70)) + IF(ISBLANK(E24),0,IF(ISNUMBER(E24),E24,60)) + IF(ISBLANK(F24),0,IF(ISNUMBER(F24),F24,30))),NA())</f>
         <v>85</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B12:B15">
-    <cfRule type="expression" dxfId="44" priority="1" stopIfTrue="1">
-      <formula>NOT(ISBLANK(B12))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17:B19">
-    <cfRule type="expression" dxfId="43" priority="21" stopIfTrue="1">
-      <formula>NOT(ISBLANK(B17))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21:B23">
-    <cfRule type="expression" dxfId="42" priority="36" stopIfTrue="1">
-      <formula>NOT(ISBLANK(B21))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12:C15">
-    <cfRule type="expression" dxfId="41" priority="2" stopIfTrue="1">
-      <formula>NOT(ISBLANK(C12))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17:C19">
-    <cfRule type="expression" dxfId="40" priority="22" stopIfTrue="1">
-      <formula>NOT(ISBLANK(C17))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21:C23">
-    <cfRule type="expression" dxfId="39" priority="37" stopIfTrue="1">
-      <formula>NOT(ISBLANK(C21))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12:D15">
-    <cfRule type="expression" dxfId="38" priority="3" stopIfTrue="1">
-      <formula>NOT(ISBLANK(D12))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17:D19">
-    <cfRule type="expression" dxfId="37" priority="23" stopIfTrue="1">
-      <formula>NOT(ISBLANK(D17))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D21:D23">
-    <cfRule type="expression" dxfId="36" priority="38" stopIfTrue="1">
-      <formula>NOT(ISBLANK(D21))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12:E15">
-    <cfRule type="expression" dxfId="35" priority="4" stopIfTrue="1">
-      <formula>NOT(ISBLANK(E12))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E17:E19">
-    <cfRule type="expression" dxfId="34" priority="24" stopIfTrue="1">
-      <formula>NOT(ISBLANK(E17))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E21:E23">
-    <cfRule type="expression" dxfId="33" priority="39" stopIfTrue="1">
-      <formula>NOT(ISBLANK(E21))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12:F15">
-    <cfRule type="expression" dxfId="32" priority="5" stopIfTrue="1">
-      <formula>NOT(ISBLANK(F12))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F17:F19">
-    <cfRule type="expression" dxfId="31" priority="25" stopIfTrue="1">
-      <formula>NOT(ISBLANK(F17))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F21:F23">
-    <cfRule type="expression" dxfId="30" priority="40" stopIfTrue="1">
-      <formula>NOT(ISBLANK(F21))</formula>
+  <conditionalFormatting sqref="D13:D16">
+    <cfRule type="expression" dxfId="56" priority="9" stopIfTrue="1">
+      <formula>NOT(ISBLANK(D13))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18:D20">
+    <cfRule type="expression" dxfId="55" priority="29" stopIfTrue="1">
+      <formula>NOT(ISBLANK(D18))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22:D24">
+    <cfRule type="expression" dxfId="54" priority="44" stopIfTrue="1">
+      <formula>NOT(ISBLANK(D22))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13:E16">
+    <cfRule type="expression" dxfId="53" priority="10" stopIfTrue="1">
+      <formula>NOT(ISBLANK(E13))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18:E20">
+    <cfRule type="expression" dxfId="52" priority="30" stopIfTrue="1">
+      <formula>NOT(ISBLANK(E18))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22:E24">
+    <cfRule type="expression" dxfId="51" priority="45" stopIfTrue="1">
+      <formula>NOT(ISBLANK(E22))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13:F16">
+    <cfRule type="expression" dxfId="50" priority="11" stopIfTrue="1">
+      <formula>NOT(ISBLANK(F13))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18:F20">
+    <cfRule type="expression" dxfId="49" priority="31" stopIfTrue="1">
+      <formula>NOT(ISBLANK(F18))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22:F24">
+    <cfRule type="expression" dxfId="48" priority="46" stopIfTrue="1">
+      <formula>NOT(ISBLANK(F22))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:B16">
+    <cfRule type="expression" dxfId="17" priority="1" stopIfTrue="1">
+      <formula>NOT(ISBLANK(B13))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:B20">
+    <cfRule type="expression" dxfId="16" priority="3" stopIfTrue="1">
+      <formula>NOT(ISBLANK(B18))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22:B24">
+    <cfRule type="expression" dxfId="15" priority="5" stopIfTrue="1">
+      <formula>NOT(ISBLANK(B22))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13:C16">
+    <cfRule type="expression" dxfId="14" priority="2" stopIfTrue="1">
+      <formula>NOT(ISBLANK(C13))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:C20">
+    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
+      <formula>NOT(ISBLANK(C18))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22:C24">
+    <cfRule type="expression" dxfId="12" priority="6" stopIfTrue="1">
+      <formula>NOT(ISBLANK(C22))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1521,13 +1678,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="50" customWidth="1"/>
     <col min="2" max="9" width="15" customWidth="1"/>
@@ -1535,12 +1692,12 @@
     <col min="11" max="15" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="22.5" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1548,7 +1705,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1556,109 +1713,105 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
-        <f>SUM(I11*30,I16*40,I20*30)/100</f>
-        <v>49.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="4" t="s">
+    </row>
+    <row r="8" spans="1:10" ht="16.899999999999999" x14ac:dyDescent="0.5">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="B8" s="4">
+        <f>IF(ISBLANK(C8),SUM(I12*30,I17*40,I21*30)/100, C8)</f>
+        <v>45</v>
+      </c>
+      <c r="C8" s="5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="C10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="D10" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="5" t="s">
+      <c r="E10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="7" t="s">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="C11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="D11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="F11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="G11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="3">
-        <f>(10 * G12 + 10 * G13 + 5 * G14 + 5 * G15) / 30</f>
+      <c r="G12" s="4">
+        <f>(10 * G13 + 10 * G14 + 5 * G15 + 5 * G16) / 30</f>
         <v>55</v>
       </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="3">
-        <f>IF(ISBLANK(H11),G11,H11)</f>
+      <c r="H12" s="13"/>
+      <c r="I12" s="4">
+        <f>IF(ISBLANK(H12),G12,H12)</f>
         <v>55</v>
-      </c>
-      <c r="J11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="13">
-        <f>IF(IF(ISBLANK(B12),0,1) + IF(ISBLANK(C12),0,1) + IF(ISBLANK(D12),0,1) + IF(ISBLANK(E12),0,1) + IF(ISBLANK(F12),0,1) = 1,IF(IF(ISBLANK(B12),0,IF(ISNUMBER(B12),B12,100)) + IF(ISBLANK(C12),0,IF(ISNUMBER(C12),C12,85)) + IF(ISBLANK(D12),0,IF(ISNUMBER(D12),D12,70)) + IF(ISBLANK(E12),0,IF(ISNUMBER(E12),E12,60)) + IF(ISBLANK(F12),0,IF(ISNUMBER(F12),F12,30)) &gt; 100, NA(), IF(ISBLANK(B12),0,IF(ISNUMBER(B12),B12,100)) + IF(ISBLANK(C12),0,IF(ISNUMBER(C12),C12,85)) + IF(ISBLANK(D12),0,IF(ISNUMBER(D12),D12,70)) + IF(ISBLANK(E12),0,IF(ISNUMBER(E12),E12,60)) + IF(ISBLANK(F12),0,IF(ISNUMBER(F12),F12,30))),NA())</f>
-        <v>60</v>
       </c>
       <c r="J12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>23</v>
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A13" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="E13" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="14">
         <f>IF(IF(ISBLANK(B13),0,1) + IF(ISBLANK(C13),0,1) + IF(ISBLANK(D13),0,1) + IF(ISBLANK(E13),0,1) + IF(ISBLANK(F13),0,1) = 1,IF(IF(ISBLANK(B13),0,IF(ISNUMBER(B13),B13,100)) + IF(ISBLANK(C13),0,IF(ISNUMBER(C13),C13,85)) + IF(ISBLANK(D13),0,IF(ISNUMBER(D13),D13,70)) + IF(ISBLANK(E13),0,IF(ISNUMBER(E13),E13,60)) + IF(ISBLANK(F13),0,IF(ISNUMBER(F13),F13,30)) &gt; 100, NA(), IF(ISBLANK(B13),0,IF(ISNUMBER(B13),B13,100)) + IF(ISBLANK(C13),0,IF(ISNUMBER(C13),C13,85)) + IF(ISBLANK(D13),0,IF(ISNUMBER(D13),D13,70)) + IF(ISBLANK(E13),0,IF(ISNUMBER(E13),E13,60)) + IF(ISBLANK(F13),0,IF(ISNUMBER(F13),F13,30))),NA())</f>
         <v>60</v>
       </c>
@@ -1666,76 +1819,76 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="13">
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="14">
         <f>IF(IF(ISBLANK(B14),0,1) + IF(ISBLANK(C14),0,1) + IF(ISBLANK(D14),0,1) + IF(ISBLANK(E14),0,1) + IF(ISBLANK(F14),0,1) = 1,IF(IF(ISBLANK(B14),0,IF(ISNUMBER(B14),B14,100)) + IF(ISBLANK(C14),0,IF(ISNUMBER(C14),C14,85)) + IF(ISBLANK(D14),0,IF(ISNUMBER(D14),D14,70)) + IF(ISBLANK(E14),0,IF(ISNUMBER(E14),E14,60)) + IF(ISBLANK(F14),0,IF(ISNUMBER(F14),F14,30)) &gt; 100, NA(), IF(ISBLANK(B14),0,IF(ISNUMBER(B14),B14,100)) + IF(ISBLANK(C14),0,IF(ISNUMBER(C14),C14,85)) + IF(ISBLANK(D14),0,IF(ISNUMBER(D14),D14,70)) + IF(ISBLANK(E14),0,IF(ISNUMBER(E14),E14,60)) + IF(ISBLANK(F14),0,IF(ISNUMBER(F14),F14,30))),NA())</f>
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="J14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="13">
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="14">
         <f>IF(IF(ISBLANK(B15),0,1) + IF(ISBLANK(C15),0,1) + IF(ISBLANK(D15),0,1) + IF(ISBLANK(E15),0,1) + IF(ISBLANK(F15),0,1) = 1,IF(IF(ISBLANK(B15),0,IF(ISNUMBER(B15),B15,100)) + IF(ISBLANK(C15),0,IF(ISNUMBER(C15),C15,85)) + IF(ISBLANK(D15),0,IF(ISNUMBER(D15),D15,70)) + IF(ISBLANK(E15),0,IF(ISNUMBER(E15),E15,60)) + IF(ISBLANK(F15),0,IF(ISNUMBER(F15),F15,30)) &gt; 100, NA(), IF(ISBLANK(B15),0,IF(ISNUMBER(B15),B15,100)) + IF(ISBLANK(C15),0,IF(ISNUMBER(C15),C15,85)) + IF(ISBLANK(D15),0,IF(ISNUMBER(D15),D15,70)) + IF(ISBLANK(E15),0,IF(ISNUMBER(E15),E15,60)) + IF(ISBLANK(F15),0,IF(ISNUMBER(F15),F15,30))),NA())</f>
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="J15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="3">
-        <f>(14 * G17 + 13 * G18 + 13 * G19) / 40</f>
-        <v>50.25</v>
-      </c>
-      <c r="H16" s="12"/>
-      <c r="I16" s="3">
-        <f>IF(ISBLANK(H16),G16,H16)</f>
-        <v>50.25</v>
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="14">
+        <f>IF(IF(ISBLANK(B16),0,1) + IF(ISBLANK(C16),0,1) + IF(ISBLANK(D16),0,1) + IF(ISBLANK(E16),0,1) + IF(ISBLANK(F16),0,1) = 1,IF(IF(ISBLANK(B16),0,IF(ISNUMBER(B16),B16,100)) + IF(ISBLANK(C16),0,IF(ISNUMBER(C16),C16,85)) + IF(ISBLANK(D16),0,IF(ISNUMBER(D16),D16,70)) + IF(ISBLANK(E16),0,IF(ISNUMBER(E16),E16,60)) + IF(ISBLANK(F16),0,IF(ISNUMBER(F16),F16,30)) &gt; 100, NA(), IF(ISBLANK(B16),0,IF(ISNUMBER(B16),B16,100)) + IF(ISBLANK(C16),0,IF(ISNUMBER(C16),C16,85)) + IF(ISBLANK(D16),0,IF(ISNUMBER(D16),D16,70)) + IF(ISBLANK(E16),0,IF(ISNUMBER(E16),E16,60)) + IF(ISBLANK(F16),0,IF(ISNUMBER(F16),F16,30))),NA())</f>
+        <v>60</v>
       </c>
       <c r="J16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="13">
-        <f>IF(IF(ISBLANK(B17),0,1) + IF(ISBLANK(C17),0,1) + IF(ISBLANK(D17),0,1) + IF(ISBLANK(E17),0,1) + IF(ISBLANK(F17),0,1) = 1,IF(IF(ISBLANK(B17),0,IF(ISNUMBER(B17),B17,100)) + IF(ISBLANK(C17),0,IF(ISNUMBER(C17),C17,85)) + IF(ISBLANK(D17),0,IF(ISNUMBER(D17),D17,70)) + IF(ISBLANK(E17),0,IF(ISNUMBER(E17),E17,60)) + IF(ISBLANK(F17),0,IF(ISNUMBER(F17),F17,30)) &gt; 100, NA(), IF(ISBLANK(B17),0,IF(ISNUMBER(B17),B17,100)) + IF(ISBLANK(C17),0,IF(ISNUMBER(C17),C17,85)) + IF(ISBLANK(D17),0,IF(ISNUMBER(D17),D17,70)) + IF(ISBLANK(E17),0,IF(ISNUMBER(E17),E17,60)) + IF(ISBLANK(F17),0,IF(ISNUMBER(F17),F17,30))),NA())</f>
-        <v>60</v>
+    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A17" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="4">
+        <f>(14 * G18 + 13 * G19 + 13 * G20) / 40</f>
+        <v>50.25</v>
+      </c>
+      <c r="H17" s="13"/>
+      <c r="I17" s="4">
+        <f>IF(ISBLANK(H17),G17,H17)</f>
+        <v>50.25</v>
       </c>
       <c r="J17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>28</v>
+    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A18" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="E18" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="14">
         <f>IF(IF(ISBLANK(B18),0,1) + IF(ISBLANK(C18),0,1) + IF(ISBLANK(D18),0,1) + IF(ISBLANK(E18),0,1) + IF(ISBLANK(F18),0,1) = 1,IF(IF(ISBLANK(B18),0,IF(ISNUMBER(B18),B18,100)) + IF(ISBLANK(C18),0,IF(ISNUMBER(C18),C18,85)) + IF(ISBLANK(D18),0,IF(ISNUMBER(D18),D18,70)) + IF(ISBLANK(E18),0,IF(ISNUMBER(E18),E18,60)) + IF(ISBLANK(F18),0,IF(ISNUMBER(F18),F18,30)) &gt; 100, NA(), IF(ISBLANK(B18),0,IF(ISNUMBER(B18),B18,100)) + IF(ISBLANK(C18),0,IF(ISNUMBER(C18),C18,85)) + IF(ISBLANK(D18),0,IF(ISNUMBER(D18),D18,70)) + IF(ISBLANK(E18),0,IF(ISNUMBER(E18),E18,60)) + IF(ISBLANK(F18),0,IF(ISNUMBER(F18),F18,30))),NA())</f>
         <v>60</v>
       </c>
@@ -1743,61 +1896,61 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" t="s">
-        <v>38</v>
-      </c>
-      <c r="G19" s="13">
+    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A19" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="14">
         <f>IF(IF(ISBLANK(B19),0,1) + IF(ISBLANK(C19),0,1) + IF(ISBLANK(D19),0,1) + IF(ISBLANK(E19),0,1) + IF(ISBLANK(F19),0,1) = 1,IF(IF(ISBLANK(B19),0,IF(ISNUMBER(B19),B19,100)) + IF(ISBLANK(C19),0,IF(ISNUMBER(C19),C19,85)) + IF(ISBLANK(D19),0,IF(ISNUMBER(D19),D19,70)) + IF(ISBLANK(E19),0,IF(ISNUMBER(E19),E19,60)) + IF(ISBLANK(F19),0,IF(ISNUMBER(F19),F19,30)) &gt; 100, NA(), IF(ISBLANK(B19),0,IF(ISNUMBER(B19),B19,100)) + IF(ISBLANK(C19),0,IF(ISNUMBER(C19),C19,85)) + IF(ISBLANK(D19),0,IF(ISNUMBER(D19),D19,70)) + IF(ISBLANK(E19),0,IF(ISNUMBER(E19),E19,60)) + IF(ISBLANK(F19),0,IF(ISNUMBER(F19),F19,30))),NA())</f>
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="J19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
+    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="14">
+        <f>IF(IF(ISBLANK(B20),0,1) + IF(ISBLANK(C20),0,1) + IF(ISBLANK(D20),0,1) + IF(ISBLANK(E20),0,1) + IF(ISBLANK(F20),0,1) = 1,IF(IF(ISBLANK(B20),0,IF(ISNUMBER(B20),B20,100)) + IF(ISBLANK(C20),0,IF(ISNUMBER(C20),C20,85)) + IF(ISBLANK(D20),0,IF(ISNUMBER(D20),D20,70)) + IF(ISBLANK(E20),0,IF(ISNUMBER(E20),E20,60)) + IF(ISBLANK(F20),0,IF(ISNUMBER(F20),F20,30)) &gt; 100, NA(), IF(ISBLANK(B20),0,IF(ISNUMBER(B20),B20,100)) + IF(ISBLANK(C20),0,IF(ISNUMBER(C20),C20,85)) + IF(ISBLANK(D20),0,IF(ISNUMBER(D20),D20,70)) + IF(ISBLANK(E20),0,IF(ISNUMBER(E20),E20,60)) + IF(ISBLANK(F20),0,IF(ISNUMBER(F20),F20,30))),NA())</f>
         <v>30</v>
-      </c>
-      <c r="G20" s="3">
-        <f>(10 * G21 + 10 * G22 + 10 * G23) / 30</f>
-        <v>43.333333333333336</v>
-      </c>
-      <c r="H20" s="12"/>
-      <c r="I20" s="3">
-        <f>IF(ISBLANK(H20),G20,H20)</f>
-        <v>43.333333333333336</v>
       </c>
       <c r="J20" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" t="s">
-        <v>38</v>
-      </c>
-      <c r="G21" s="13">
-        <f>IF(IF(ISBLANK(B21),0,1) + IF(ISBLANK(C21),0,1) + IF(ISBLANK(D21),0,1) + IF(ISBLANK(E21),0,1) + IF(ISBLANK(F21),0,1) = 1,IF(IF(ISBLANK(B21),0,IF(ISNUMBER(B21),B21,100)) + IF(ISBLANK(C21),0,IF(ISNUMBER(C21),C21,85)) + IF(ISBLANK(D21),0,IF(ISNUMBER(D21),D21,70)) + IF(ISBLANK(E21),0,IF(ISNUMBER(E21),E21,60)) + IF(ISBLANK(F21),0,IF(ISNUMBER(F21),F21,30)) &gt; 100, NA(), IF(ISBLANK(B21),0,IF(ISNUMBER(B21),B21,100)) + IF(ISBLANK(C21),0,IF(ISNUMBER(C21),C21,85)) + IF(ISBLANK(D21),0,IF(ISNUMBER(D21),D21,70)) + IF(ISBLANK(E21),0,IF(ISNUMBER(E21),E21,60)) + IF(ISBLANK(F21),0,IF(ISNUMBER(F21),F21,30))),NA())</f>
+    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A21" s="12" t="s">
         <v>30</v>
+      </c>
+      <c r="G21" s="4">
+        <f>(10 * G22 + 10 * G23 + 10 * G24) / 30</f>
+        <v>43.333333333333336</v>
+      </c>
+      <c r="H21" s="13"/>
+      <c r="I21" s="4">
+        <f>IF(ISBLANK(H21),G21,H21)</f>
+        <v>43.333333333333336</v>
       </c>
       <c r="J21" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>32</v>
+    <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A22" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="F22" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="14">
         <f>IF(IF(ISBLANK(B22),0,1) + IF(ISBLANK(C22),0,1) + IF(ISBLANK(D22),0,1) + IF(ISBLANK(E22),0,1) + IF(ISBLANK(F22),0,1) = 1,IF(IF(ISBLANK(B22),0,IF(ISNUMBER(B22),B22,100)) + IF(ISBLANK(C22),0,IF(ISNUMBER(C22),C22,85)) + IF(ISBLANK(D22),0,IF(ISNUMBER(D22),D22,70)) + IF(ISBLANK(E22),0,IF(ISNUMBER(E22),E22,60)) + IF(ISBLANK(F22),0,IF(ISNUMBER(F22),F22,30)) &gt; 100, NA(), IF(ISBLANK(B22),0,IF(ISNUMBER(B22),B22,100)) + IF(ISBLANK(C22),0,IF(ISNUMBER(C22),C22,85)) + IF(ISBLANK(D22),0,IF(ISNUMBER(D22),D22,70)) + IF(ISBLANK(E22),0,IF(ISNUMBER(E22),E22,60)) + IF(ISBLANK(F22),0,IF(ISNUMBER(F22),F22,30))),NA())</f>
         <v>30</v>
       </c>
@@ -1805,95 +1958,110 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" s="13">
+    <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A23" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="14">
         <f>IF(IF(ISBLANK(B23),0,1) + IF(ISBLANK(C23),0,1) + IF(ISBLANK(D23),0,1) + IF(ISBLANK(E23),0,1) + IF(ISBLANK(F23),0,1) = 1,IF(IF(ISBLANK(B23),0,IF(ISNUMBER(B23),B23,100)) + IF(ISBLANK(C23),0,IF(ISNUMBER(C23),C23,85)) + IF(ISBLANK(D23),0,IF(ISNUMBER(D23),D23,70)) + IF(ISBLANK(E23),0,IF(ISNUMBER(E23),E23,60)) + IF(ISBLANK(F23),0,IF(ISNUMBER(F23),F23,30)) &gt; 100, NA(), IF(ISBLANK(B23),0,IF(ISNUMBER(B23),B23,100)) + IF(ISBLANK(C23),0,IF(ISNUMBER(C23),C23,85)) + IF(ISBLANK(D23),0,IF(ISNUMBER(D23),D23,70)) + IF(ISBLANK(E23),0,IF(ISNUMBER(E23),E23,60)) + IF(ISBLANK(F23),0,IF(ISNUMBER(F23),F23,30))),NA())</f>
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="J23" t="s">
         <v>55</v>
       </c>
     </row>
+    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="14">
+        <f>IF(IF(ISBLANK(B24),0,1) + IF(ISBLANK(C24),0,1) + IF(ISBLANK(D24),0,1) + IF(ISBLANK(E24),0,1) + IF(ISBLANK(F24),0,1) = 1,IF(IF(ISBLANK(B24),0,IF(ISNUMBER(B24),B24,100)) + IF(ISBLANK(C24),0,IF(ISNUMBER(C24),C24,85)) + IF(ISBLANK(D24),0,IF(ISNUMBER(D24),D24,70)) + IF(ISBLANK(E24),0,IF(ISNUMBER(E24),E24,60)) + IF(ISBLANK(F24),0,IF(ISNUMBER(F24),F24,30)) &gt; 100, NA(), IF(ISBLANK(B24),0,IF(ISNUMBER(B24),B24,100)) + IF(ISBLANK(C24),0,IF(ISNUMBER(C24),C24,85)) + IF(ISBLANK(D24),0,IF(ISNUMBER(D24),D24,70)) + IF(ISBLANK(E24),0,IF(ISNUMBER(E24),E24,60)) + IF(ISBLANK(F24),0,IF(ISNUMBER(F24),F24,30))),NA())</f>
+        <v>70</v>
+      </c>
+      <c r="J24" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B12:B15">
-    <cfRule type="expression" dxfId="29" priority="1" stopIfTrue="1">
-      <formula>NOT(ISBLANK(B12))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17:B19">
-    <cfRule type="expression" dxfId="28" priority="21" stopIfTrue="1">
-      <formula>NOT(ISBLANK(B17))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21:B23">
-    <cfRule type="expression" dxfId="27" priority="36" stopIfTrue="1">
-      <formula>NOT(ISBLANK(B21))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12:C15">
-    <cfRule type="expression" dxfId="26" priority="2" stopIfTrue="1">
-      <formula>NOT(ISBLANK(C12))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17:C19">
-    <cfRule type="expression" dxfId="25" priority="22" stopIfTrue="1">
-      <formula>NOT(ISBLANK(C17))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21:C23">
-    <cfRule type="expression" dxfId="24" priority="37" stopIfTrue="1">
-      <formula>NOT(ISBLANK(C21))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12:D15">
-    <cfRule type="expression" dxfId="23" priority="3" stopIfTrue="1">
-      <formula>NOT(ISBLANK(D12))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17:D19">
-    <cfRule type="expression" dxfId="22" priority="23" stopIfTrue="1">
-      <formula>NOT(ISBLANK(D17))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D21:D23">
-    <cfRule type="expression" dxfId="21" priority="38" stopIfTrue="1">
-      <formula>NOT(ISBLANK(D21))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12:E15">
-    <cfRule type="expression" dxfId="20" priority="4" stopIfTrue="1">
-      <formula>NOT(ISBLANK(E12))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E17:E19">
-    <cfRule type="expression" dxfId="19" priority="24" stopIfTrue="1">
-      <formula>NOT(ISBLANK(E17))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E21:E23">
-    <cfRule type="expression" dxfId="18" priority="39" stopIfTrue="1">
-      <formula>NOT(ISBLANK(E21))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12:F15">
-    <cfRule type="expression" dxfId="17" priority="5" stopIfTrue="1">
-      <formula>NOT(ISBLANK(F12))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F17:F19">
-    <cfRule type="expression" dxfId="16" priority="25" stopIfTrue="1">
-      <formula>NOT(ISBLANK(F17))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F21:F23">
-    <cfRule type="expression" dxfId="15" priority="40" stopIfTrue="1">
-      <formula>NOT(ISBLANK(F21))</formula>
+  <conditionalFormatting sqref="B13:B16">
+    <cfRule type="expression" dxfId="47" priority="10" stopIfTrue="1">
+      <formula>NOT(ISBLANK(B13))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:B20">
+    <cfRule type="expression" dxfId="46" priority="30" stopIfTrue="1">
+      <formula>NOT(ISBLANK(B18))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22:B24">
+    <cfRule type="expression" dxfId="45" priority="45" stopIfTrue="1">
+      <formula>NOT(ISBLANK(B22))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13:C16">
+    <cfRule type="expression" dxfId="44" priority="11" stopIfTrue="1">
+      <formula>NOT(ISBLANK(C13))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:C20">
+    <cfRule type="expression" dxfId="43" priority="31" stopIfTrue="1">
+      <formula>NOT(ISBLANK(C18))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22:C24">
+    <cfRule type="expression" dxfId="42" priority="46" stopIfTrue="1">
+      <formula>NOT(ISBLANK(C22))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13:D16">
+    <cfRule type="expression" dxfId="11" priority="1" stopIfTrue="1">
+      <formula>NOT(ISBLANK(D13))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18:D20">
+    <cfRule type="expression" dxfId="10" priority="4" stopIfTrue="1">
+      <formula>NOT(ISBLANK(D18))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22:D24">
+    <cfRule type="expression" dxfId="9" priority="7" stopIfTrue="1">
+      <formula>NOT(ISBLANK(D22))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13:E16">
+    <cfRule type="expression" dxfId="8" priority="2" stopIfTrue="1">
+      <formula>NOT(ISBLANK(E13))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18:E20">
+    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
+      <formula>NOT(ISBLANK(E18))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22:E24">
+    <cfRule type="expression" dxfId="6" priority="8" stopIfTrue="1">
+      <formula>NOT(ISBLANK(E22))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13:F16">
+    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+      <formula>NOT(ISBLANK(F13))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18:F20">
+    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
+      <formula>NOT(ISBLANK(F18))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22:F24">
+    <cfRule type="expression" dxfId="3" priority="9" stopIfTrue="1">
+      <formula>NOT(ISBLANK(F22))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1902,13 +2070,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="50" customWidth="1"/>
     <col min="2" max="9" width="15" customWidth="1"/>
@@ -1916,12 +2084,12 @@
     <col min="11" max="15" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="22.5" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1929,7 +2097,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1937,7 +2105,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1945,297 +2113,306 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
-        <f>SUM(I11*30,I16*40,I20*30)/100</f>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="16.899999999999999" x14ac:dyDescent="0.5">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4">
+        <f>IF(ISBLANK(C8),SUM(I12*30,I17*40,I21*30)/100, C8)</f>
         <v>85</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
+      <c r="C8" s="5"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="10" t="s">
+      <c r="I11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="3">
-        <f>(10 * G12 + 10 * G13 + 5 * G14 + 5 * G15) / 30</f>
+      <c r="G12" s="4">
+        <f>(10 * G13 + 10 * G14 + 5 * G15 + 5 * G16) / 30</f>
         <v>85</v>
       </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="3">
-        <f>IF(ISBLANK(H11),G11,H11)</f>
+      <c r="H12" s="13"/>
+      <c r="I12" s="4">
+        <f>IF(ISBLANK(H12),G12,H12)</f>
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="13">
-        <f>IF(IF(ISBLANK(B12),0,1) + IF(ISBLANK(C12),0,1) + IF(ISBLANK(D12),0,1) + IF(ISBLANK(E12),0,1) + IF(ISBLANK(F12),0,1) = 1,IF(IF(ISBLANK(B12),0,IF(ISNUMBER(B12),B12,100)) + IF(ISBLANK(C12),0,IF(ISNUMBER(C12),C12,85)) + IF(ISBLANK(D12),0,IF(ISNUMBER(D12),D12,70)) + IF(ISBLANK(E12),0,IF(ISNUMBER(E12),E12,60)) + IF(ISBLANK(F12),0,IF(ISNUMBER(F12),F12,30)) &gt; 100, NA(), IF(ISBLANK(B12),0,IF(ISNUMBER(B12),B12,100)) + IF(ISBLANK(C12),0,IF(ISNUMBER(C12),C12,85)) + IF(ISBLANK(D12),0,IF(ISNUMBER(D12),D12,70)) + IF(ISBLANK(E12),0,IF(ISNUMBER(E12),E12,60)) + IF(ISBLANK(F12),0,IF(ISNUMBER(F12),F12,30))),NA())</f>
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="C13" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="14">
         <f>IF(IF(ISBLANK(B13),0,1) + IF(ISBLANK(C13),0,1) + IF(ISBLANK(D13),0,1) + IF(ISBLANK(E13),0,1) + IF(ISBLANK(F13),0,1) = 1,IF(IF(ISBLANK(B13),0,IF(ISNUMBER(B13),B13,100)) + IF(ISBLANK(C13),0,IF(ISNUMBER(C13),C13,85)) + IF(ISBLANK(D13),0,IF(ISNUMBER(D13),D13,70)) + IF(ISBLANK(E13),0,IF(ISNUMBER(E13),E13,60)) + IF(ISBLANK(F13),0,IF(ISNUMBER(F13),F13,30)) &gt; 100, NA(), IF(ISBLANK(B13),0,IF(ISNUMBER(B13),B13,100)) + IF(ISBLANK(C13),0,IF(ISNUMBER(C13),C13,85)) + IF(ISBLANK(D13),0,IF(ISNUMBER(D13),D13,70)) + IF(ISBLANK(E13),0,IF(ISNUMBER(E13),E13,60)) + IF(ISBLANK(F13),0,IF(ISNUMBER(F13),F13,30))),NA())</f>
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>24</v>
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A14" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="14">
         <f>IF(IF(ISBLANK(B14),0,1) + IF(ISBLANK(C14),0,1) + IF(ISBLANK(D14),0,1) + IF(ISBLANK(E14),0,1) + IF(ISBLANK(F14),0,1) = 1,IF(IF(ISBLANK(B14),0,IF(ISNUMBER(B14),B14,100)) + IF(ISBLANK(C14),0,IF(ISNUMBER(C14),C14,85)) + IF(ISBLANK(D14),0,IF(ISNUMBER(D14),D14,70)) + IF(ISBLANK(E14),0,IF(ISNUMBER(E14),E14,60)) + IF(ISBLANK(F14),0,IF(ISNUMBER(F14),F14,30)) &gt; 100, NA(), IF(ISBLANK(B14),0,IF(ISNUMBER(B14),B14,100)) + IF(ISBLANK(C14),0,IF(ISNUMBER(C14),C14,85)) + IF(ISBLANK(D14),0,IF(ISNUMBER(D14),D14,70)) + IF(ISBLANK(E14),0,IF(ISNUMBER(E14),E14,60)) + IF(ISBLANK(F14),0,IF(ISNUMBER(F14),F14,30))),NA())</f>
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>25</v>
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A15" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="C15" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="14">
         <f>IF(IF(ISBLANK(B15),0,1) + IF(ISBLANK(C15),0,1) + IF(ISBLANK(D15),0,1) + IF(ISBLANK(E15),0,1) + IF(ISBLANK(F15),0,1) = 1,IF(IF(ISBLANK(B15),0,IF(ISNUMBER(B15),B15,100)) + IF(ISBLANK(C15),0,IF(ISNUMBER(C15),C15,85)) + IF(ISBLANK(D15),0,IF(ISNUMBER(D15),D15,70)) + IF(ISBLANK(E15),0,IF(ISNUMBER(E15),E15,60)) + IF(ISBLANK(F15),0,IF(ISNUMBER(F15),F15,30)) &gt; 100, NA(), IF(ISBLANK(B15),0,IF(ISNUMBER(B15),B15,100)) + IF(ISBLANK(C15),0,IF(ISNUMBER(C15),C15,85)) + IF(ISBLANK(D15),0,IF(ISNUMBER(D15),D15,70)) + IF(ISBLANK(E15),0,IF(ISNUMBER(E15),E15,60)) + IF(ISBLANK(F15),0,IF(ISNUMBER(F15),F15,30))),NA())</f>
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="14">
+        <f>IF(IF(ISBLANK(B16),0,1) + IF(ISBLANK(C16),0,1) + IF(ISBLANK(D16),0,1) + IF(ISBLANK(E16),0,1) + IF(ISBLANK(F16),0,1) = 1,IF(IF(ISBLANK(B16),0,IF(ISNUMBER(B16),B16,100)) + IF(ISBLANK(C16),0,IF(ISNUMBER(C16),C16,85)) + IF(ISBLANK(D16),0,IF(ISNUMBER(D16),D16,70)) + IF(ISBLANK(E16),0,IF(ISNUMBER(E16),E16,60)) + IF(ISBLANK(F16),0,IF(ISNUMBER(F16),F16,30)) &gt; 100, NA(), IF(ISBLANK(B16),0,IF(ISNUMBER(B16),B16,100)) + IF(ISBLANK(C16),0,IF(ISNUMBER(C16),C16,85)) + IF(ISBLANK(D16),0,IF(ISNUMBER(D16),D16,70)) + IF(ISBLANK(E16),0,IF(ISNUMBER(E16),E16,60)) + IF(ISBLANK(F16),0,IF(ISNUMBER(F16),F16,30))),NA())</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A17" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="3">
-        <f>(14 * G17 + 13 * G18 + 13 * G19) / 40</f>
+      <c r="G17" s="4">
+        <f>(14 * G18 + 13 * G19 + 13 * G20) / 40</f>
         <v>85</v>
       </c>
-      <c r="H16" s="12"/>
-      <c r="I16" s="3">
-        <f>IF(ISBLANK(H16),G16,H16)</f>
+      <c r="H17" s="13"/>
+      <c r="I17" s="4">
+        <f>IF(ISBLANK(H17),G17,H17)</f>
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C17" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="13">
-        <f>IF(IF(ISBLANK(B17),0,1) + IF(ISBLANK(C17),0,1) + IF(ISBLANK(D17),0,1) + IF(ISBLANK(E17),0,1) + IF(ISBLANK(F17),0,1) = 1,IF(IF(ISBLANK(B17),0,IF(ISNUMBER(B17),B17,100)) + IF(ISBLANK(C17),0,IF(ISNUMBER(C17),C17,85)) + IF(ISBLANK(D17),0,IF(ISNUMBER(D17),D17,70)) + IF(ISBLANK(E17),0,IF(ISNUMBER(E17),E17,60)) + IF(ISBLANK(F17),0,IF(ISNUMBER(F17),F17,30)) &gt; 100, NA(), IF(ISBLANK(B17),0,IF(ISNUMBER(B17),B17,100)) + IF(ISBLANK(C17),0,IF(ISNUMBER(C17),C17,85)) + IF(ISBLANK(D17),0,IF(ISNUMBER(D17),D17,70)) + IF(ISBLANK(E17),0,IF(ISNUMBER(E17),E17,60)) + IF(ISBLANK(F17),0,IF(ISNUMBER(F17),F17,30))),NA())</f>
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="C18" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="14">
         <f>IF(IF(ISBLANK(B18),0,1) + IF(ISBLANK(C18),0,1) + IF(ISBLANK(D18),0,1) + IF(ISBLANK(E18),0,1) + IF(ISBLANK(F18),0,1) = 1,IF(IF(ISBLANK(B18),0,IF(ISNUMBER(B18),B18,100)) + IF(ISBLANK(C18),0,IF(ISNUMBER(C18),C18,85)) + IF(ISBLANK(D18),0,IF(ISNUMBER(D18),D18,70)) + IF(ISBLANK(E18),0,IF(ISNUMBER(E18),E18,60)) + IF(ISBLANK(F18),0,IF(ISNUMBER(F18),F18,30)) &gt; 100, NA(), IF(ISBLANK(B18),0,IF(ISNUMBER(B18),B18,100)) + IF(ISBLANK(C18),0,IF(ISNUMBER(C18),C18,85)) + IF(ISBLANK(D18),0,IF(ISNUMBER(D18),D18,70)) + IF(ISBLANK(E18),0,IF(ISNUMBER(E18),E18,60)) + IF(ISBLANK(F18),0,IF(ISNUMBER(F18),F18,30))),NA())</f>
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>29</v>
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A19" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="C19" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="14">
         <f>IF(IF(ISBLANK(B19),0,1) + IF(ISBLANK(C19),0,1) + IF(ISBLANK(D19),0,1) + IF(ISBLANK(E19),0,1) + IF(ISBLANK(F19),0,1) = 1,IF(IF(ISBLANK(B19),0,IF(ISNUMBER(B19),B19,100)) + IF(ISBLANK(C19),0,IF(ISNUMBER(C19),C19,85)) + IF(ISBLANK(D19),0,IF(ISNUMBER(D19),D19,70)) + IF(ISBLANK(E19),0,IF(ISNUMBER(E19),E19,60)) + IF(ISBLANK(F19),0,IF(ISNUMBER(F19),F19,30)) &gt; 100, NA(), IF(ISBLANK(B19),0,IF(ISNUMBER(B19),B19,100)) + IF(ISBLANK(C19),0,IF(ISNUMBER(C19),C19,85)) + IF(ISBLANK(D19),0,IF(ISNUMBER(D19),D19,70)) + IF(ISBLANK(E19),0,IF(ISNUMBER(E19),E19,60)) + IF(ISBLANK(F19),0,IF(ISNUMBER(F19),F19,30))),NA())</f>
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="14">
+        <f>IF(IF(ISBLANK(B20),0,1) + IF(ISBLANK(C20),0,1) + IF(ISBLANK(D20),0,1) + IF(ISBLANK(E20),0,1) + IF(ISBLANK(F20),0,1) = 1,IF(IF(ISBLANK(B20),0,IF(ISNUMBER(B20),B20,100)) + IF(ISBLANK(C20),0,IF(ISNUMBER(C20),C20,85)) + IF(ISBLANK(D20),0,IF(ISNUMBER(D20),D20,70)) + IF(ISBLANK(E20),0,IF(ISNUMBER(E20),E20,60)) + IF(ISBLANK(F20),0,IF(ISNUMBER(F20),F20,30)) &gt; 100, NA(), IF(ISBLANK(B20),0,IF(ISNUMBER(B20),B20,100)) + IF(ISBLANK(C20),0,IF(ISNUMBER(C20),C20,85)) + IF(ISBLANK(D20),0,IF(ISNUMBER(D20),D20,70)) + IF(ISBLANK(E20),0,IF(ISNUMBER(E20),E20,60)) + IF(ISBLANK(F20),0,IF(ISNUMBER(F20),F20,30))),NA())</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A21" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="3">
-        <f>(10 * G21 + 10 * G22 + 10 * G23) / 30</f>
+      <c r="G21" s="4">
+        <f>(10 * G22 + 10 * G23 + 10 * G24) / 30</f>
         <v>85</v>
       </c>
-      <c r="H20" s="12"/>
-      <c r="I20" s="3">
-        <f>IF(ISBLANK(H20),G20,H20)</f>
+      <c r="H21" s="13"/>
+      <c r="I21" s="4">
+        <f>IF(ISBLANK(H21),G21,H21)</f>
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A22" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C21" t="s">
-        <v>38</v>
-      </c>
-      <c r="G21" s="13">
-        <f>IF(IF(ISBLANK(B21),0,1) + IF(ISBLANK(C21),0,1) + IF(ISBLANK(D21),0,1) + IF(ISBLANK(E21),0,1) + IF(ISBLANK(F21),0,1) = 1,IF(IF(ISBLANK(B21),0,IF(ISNUMBER(B21),B21,100)) + IF(ISBLANK(C21),0,IF(ISNUMBER(C21),C21,85)) + IF(ISBLANK(D21),0,IF(ISNUMBER(D21),D21,70)) + IF(ISBLANK(E21),0,IF(ISNUMBER(E21),E21,60)) + IF(ISBLANK(F21),0,IF(ISNUMBER(F21),F21,30)) &gt; 100, NA(), IF(ISBLANK(B21),0,IF(ISNUMBER(B21),B21,100)) + IF(ISBLANK(C21),0,IF(ISNUMBER(C21),C21,85)) + IF(ISBLANK(D21),0,IF(ISNUMBER(D21),D21,70)) + IF(ISBLANK(E21),0,IF(ISNUMBER(E21),E21,60)) + IF(ISBLANK(F21),0,IF(ISNUMBER(F21),F21,30))),NA())</f>
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="C22" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="14">
         <f>IF(IF(ISBLANK(B22),0,1) + IF(ISBLANK(C22),0,1) + IF(ISBLANK(D22),0,1) + IF(ISBLANK(E22),0,1) + IF(ISBLANK(F22),0,1) = 1,IF(IF(ISBLANK(B22),0,IF(ISNUMBER(B22),B22,100)) + IF(ISBLANK(C22),0,IF(ISNUMBER(C22),C22,85)) + IF(ISBLANK(D22),0,IF(ISNUMBER(D22),D22,70)) + IF(ISBLANK(E22),0,IF(ISNUMBER(E22),E22,60)) + IF(ISBLANK(F22),0,IF(ISNUMBER(F22),F22,30)) &gt; 100, NA(), IF(ISBLANK(B22),0,IF(ISNUMBER(B22),B22,100)) + IF(ISBLANK(C22),0,IF(ISNUMBER(C22),C22,85)) + IF(ISBLANK(D22),0,IF(ISNUMBER(D22),D22,70)) + IF(ISBLANK(E22),0,IF(ISNUMBER(E22),E22,60)) + IF(ISBLANK(F22),0,IF(ISNUMBER(F22),F22,30))),NA())</f>
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>33</v>
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A23" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="C23" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="13">
+      <c r="G23" s="14">
         <f>IF(IF(ISBLANK(B23),0,1) + IF(ISBLANK(C23),0,1) + IF(ISBLANK(D23),0,1) + IF(ISBLANK(E23),0,1) + IF(ISBLANK(F23),0,1) = 1,IF(IF(ISBLANK(B23),0,IF(ISNUMBER(B23),B23,100)) + IF(ISBLANK(C23),0,IF(ISNUMBER(C23),C23,85)) + IF(ISBLANK(D23),0,IF(ISNUMBER(D23),D23,70)) + IF(ISBLANK(E23),0,IF(ISNUMBER(E23),E23,60)) + IF(ISBLANK(F23),0,IF(ISNUMBER(F23),F23,30)) &gt; 100, NA(), IF(ISBLANK(B23),0,IF(ISNUMBER(B23),B23,100)) + IF(ISBLANK(C23),0,IF(ISNUMBER(C23),C23,85)) + IF(ISBLANK(D23),0,IF(ISNUMBER(D23),D23,70)) + IF(ISBLANK(E23),0,IF(ISNUMBER(E23),E23,60)) + IF(ISBLANK(F23),0,IF(ISNUMBER(F23),F23,30))),NA())</f>
         <v>85</v>
       </c>
     </row>
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="14">
+        <f>IF(IF(ISBLANK(B24),0,1) + IF(ISBLANK(C24),0,1) + IF(ISBLANK(D24),0,1) + IF(ISBLANK(E24),0,1) + IF(ISBLANK(F24),0,1) = 1,IF(IF(ISBLANK(B24),0,IF(ISNUMBER(B24),B24,100)) + IF(ISBLANK(C24),0,IF(ISNUMBER(C24),C24,85)) + IF(ISBLANK(D24),0,IF(ISNUMBER(D24),D24,70)) + IF(ISBLANK(E24),0,IF(ISNUMBER(E24),E24,60)) + IF(ISBLANK(F24),0,IF(ISNUMBER(F24),F24,30)) &gt; 100, NA(), IF(ISBLANK(B24),0,IF(ISNUMBER(B24),B24,100)) + IF(ISBLANK(C24),0,IF(ISNUMBER(C24),C24,85)) + IF(ISBLANK(D24),0,IF(ISNUMBER(D24),D24,70)) + IF(ISBLANK(E24),0,IF(ISNUMBER(E24),E24,60)) + IF(ISBLANK(F24),0,IF(ISNUMBER(F24),F24,30))),NA())</f>
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B12:B15">
-    <cfRule type="expression" dxfId="14" priority="1" stopIfTrue="1">
-      <formula>NOT(ISBLANK(B12))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17:B19">
-    <cfRule type="expression" dxfId="13" priority="21" stopIfTrue="1">
-      <formula>NOT(ISBLANK(B17))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21:B23">
-    <cfRule type="expression" dxfId="12" priority="36" stopIfTrue="1">
-      <formula>NOT(ISBLANK(B21))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12:C15">
-    <cfRule type="expression" dxfId="11" priority="2" stopIfTrue="1">
-      <formula>NOT(ISBLANK(C12))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17:C19">
-    <cfRule type="expression" dxfId="10" priority="22" stopIfTrue="1">
-      <formula>NOT(ISBLANK(C17))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21:C23">
-    <cfRule type="expression" dxfId="9" priority="37" stopIfTrue="1">
-      <formula>NOT(ISBLANK(C21))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12:D15">
-    <cfRule type="expression" dxfId="8" priority="3" stopIfTrue="1">
-      <formula>NOT(ISBLANK(D12))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17:D19">
-    <cfRule type="expression" dxfId="7" priority="23" stopIfTrue="1">
-      <formula>NOT(ISBLANK(D17))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D21:D23">
-    <cfRule type="expression" dxfId="6" priority="38" stopIfTrue="1">
-      <formula>NOT(ISBLANK(D21))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12:E15">
-    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
-      <formula>NOT(ISBLANK(E12))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E17:E19">
-    <cfRule type="expression" dxfId="4" priority="24" stopIfTrue="1">
-      <formula>NOT(ISBLANK(E17))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E21:E23">
-    <cfRule type="expression" dxfId="3" priority="39" stopIfTrue="1">
-      <formula>NOT(ISBLANK(E21))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12:F15">
-    <cfRule type="expression" dxfId="2" priority="5" stopIfTrue="1">
-      <formula>NOT(ISBLANK(F12))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F17:F19">
-    <cfRule type="expression" dxfId="1" priority="25" stopIfTrue="1">
-      <formula>NOT(ISBLANK(F17))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F21:F23">
-    <cfRule type="expression" dxfId="0" priority="40" stopIfTrue="1">
-      <formula>NOT(ISBLANK(F21))</formula>
+  <conditionalFormatting sqref="B13:B16">
+    <cfRule type="expression" dxfId="32" priority="4" stopIfTrue="1">
+      <formula>NOT(ISBLANK(B13))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:B20">
+    <cfRule type="expression" dxfId="31" priority="24" stopIfTrue="1">
+      <formula>NOT(ISBLANK(B18))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22:B24">
+    <cfRule type="expression" dxfId="30" priority="39" stopIfTrue="1">
+      <formula>NOT(ISBLANK(B22))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13:D16">
+    <cfRule type="expression" dxfId="26" priority="6" stopIfTrue="1">
+      <formula>NOT(ISBLANK(D13))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18:D20">
+    <cfRule type="expression" dxfId="25" priority="26" stopIfTrue="1">
+      <formula>NOT(ISBLANK(D18))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22:D24">
+    <cfRule type="expression" dxfId="24" priority="41" stopIfTrue="1">
+      <formula>NOT(ISBLANK(D22))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13:E16">
+    <cfRule type="expression" dxfId="23" priority="7" stopIfTrue="1">
+      <formula>NOT(ISBLANK(E13))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18:E20">
+    <cfRule type="expression" dxfId="22" priority="27" stopIfTrue="1">
+      <formula>NOT(ISBLANK(E18))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22:E24">
+    <cfRule type="expression" dxfId="21" priority="42" stopIfTrue="1">
+      <formula>NOT(ISBLANK(E22))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13:F16">
+    <cfRule type="expression" dxfId="20" priority="8" stopIfTrue="1">
+      <formula>NOT(ISBLANK(F13))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18:F20">
+    <cfRule type="expression" dxfId="19" priority="28" stopIfTrue="1">
+      <formula>NOT(ISBLANK(F18))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22:F24">
+    <cfRule type="expression" dxfId="18" priority="43" stopIfTrue="1">
+      <formula>NOT(ISBLANK(F22))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13:C16">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+      <formula>NOT(ISBLANK(C13))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:C20">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+      <formula>NOT(ISBLANK(C18))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22:C24">
+    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
+      <formula>NOT(ISBLANK(C22))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add GradeSheet, simplify Indicator, Criterion and Evaluation
</commit_message>
<xml_diff>
--- a/tests/fixtures/grille_gradebook.xlsx
+++ b/tests/fixtures/grille_gradebook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varch\Git-repos\c3hm\tests\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D41E1FE-86B8-4AAD-AC49-C851B8E472E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B335E7-DA69-47B8-BB09-288EBAAA135E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27982" yWindow="360" windowWidth="27247" windowHeight="14738" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27953" yWindow="428" windowWidth="27248" windowHeight="14737" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="houle" sheetId="1" r:id="rId1"/>
@@ -403,7 +403,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -1702,7 +1702,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1926,15 +1926,15 @@
       <c r="D15" s="13"/>
       <c r="E15" s="14">
         <f>F15 / 40</f>
-        <v>0.75</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="F15" s="15">
         <f>IF(AND(NOT(ISBLANK(B15)),NOT(ISBLANK(C15))), NA(), IF(NOT(ISBLANK(B15)),B15 * 40,IF(NOT(ISBLANK(C15)),C15, SUM(cthm_C2_I1_points, cthm_C2_I2_points, cthm_C2_I3_points))))</f>
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="G15" s="15" t="str">
         <f>IF(cthm_C2_points / 40 &gt;= 0.9,"Excellent", IF(cthm_C2_points / 40 &gt;= 0.8,"Très bien", IF(cthm_C2_points / 40 &gt;= 0.7,"Bien", IF(cthm_C2_points / 40 &gt;= 0.6,"Passable", IF(cthm_C2_points / 40 &gt;= 0,"Insuffisant", "")))))</f>
-        <v>Bien</v>
+        <v>Excellent</v>
       </c>
       <c r="H15" s="7"/>
     </row>
@@ -1942,72 +1942,75 @@
       <c r="A16" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="5">
-        <v>0.75</v>
+      <c r="B16" s="5"/>
+      <c r="C16">
+        <v>13</v>
       </c>
       <c r="E16" s="9">
         <f>F16 / 14</f>
-        <v>0.75</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="F16" s="10">
         <f>IF(AND(NOT(ISBLANK(B16)),NOT(ISBLANK(C16))), NA(), IF(NOT(ISBLANK(B16)),B16 * 14,IF(NOT(ISBLANK(C16)),C16, NA())))</f>
-        <v>10.5</v>
+        <v>13</v>
       </c>
       <c r="G16" s="10" t="str">
         <f>IF(cthm_C2_I1_points / 14 &gt;= 0.9,"Excellent", IF(cthm_C2_I1_points / 14 &gt;= 0.8,"Très bien", IF(cthm_C2_I1_points / 14 &gt;= 0.7,"Bien", IF(cthm_C2_I1_points / 14 &gt;= 0.6,"Passable", IF(cthm_C2_I1_points / 14 &gt;= 0,"Insuffisant", "")))))</f>
-        <v>Bien</v>
+        <v>Excellent</v>
       </c>
       <c r="H16" s="10" t="str">
         <f>IF(cthm_C2_I1_points / 14 &gt;= 0.9,"Nœud huit parfait, digne d’un musée des beaux cordages !", IF(cthm_C2_I1_points / 14 &gt;= 0.8,"Tours bien placés, un seul brin chevauche légèrement.", IF(cthm_C2_I1_points / 14 &gt;= 0.7,"Structure correcte mais cordage un peu lâche.", IF(cthm_C2_I1_points / 14 &gt;= 0.6,"Hésitations visibles, le huit part en vrille.", IF(cthm_C2_I1_points / 14 &gt;= 0,"Corde en salade, impossible à démêler sans un bon couteau.", "")))))</f>
-        <v>Structure correcte mais cordage un peu lâche.</v>
+        <v>Nœud huit parfait, digne d’un musée des beaux cordages !</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="5">
-        <v>0.75</v>
+      <c r="B17" s="5"/>
+      <c r="C17">
+        <v>13</v>
       </c>
       <c r="E17" s="9">
         <f>F17 / 13</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F17" s="10">
         <f>IF(AND(NOT(ISBLANK(B17)),NOT(ISBLANK(C17))), NA(), IF(NOT(ISBLANK(B17)),B17 * 13,IF(NOT(ISBLANK(C17)),C17, NA())))</f>
-        <v>9.75</v>
+        <v>13</v>
       </c>
       <c r="G17" s="10" t="str">
         <f>IF(cthm_C2_I2_points / 13 &gt;= 0.9,"Excellent", IF(cthm_C2_I2_points / 13 &gt;= 0.8,"Très bien", IF(cthm_C2_I2_points / 13 &gt;= 0.7,"Bien", IF(cthm_C2_I2_points / 13 &gt;= 0.6,"Passable", IF(cthm_C2_I2_points / 13 &gt;= 0,"Insuffisant", "")))))</f>
-        <v>Bien</v>
+        <v>Excellent</v>
       </c>
       <c r="H17" s="10" t="str">
         <f>IF(cthm_C2_I2_points / 13 &gt;= 0.9,"Le drapeau claque fièrement, aucun risque de le voir s’envoler.", IF(cthm_C2_I2_points / 13 &gt;= 0.8,"Fixation robuste, léger flottement par grands vents.", IF(cthm_C2_I2_points / 13 &gt;= 0.7,"Accroché convenablement, mais se relâche parfois.", IF(cthm_C2_I2_points / 13 &gt;= 0.6,"Pavillon branlant, mauvais signe pour la détermination.", IF(cthm_C2_I2_points / 13 &gt;= 0,"Pendouille misérablement, honneur entamé.", "")))))</f>
-        <v>Accroché convenablement, mais se relâche parfois.</v>
+        <v>Le drapeau claque fièrement, aucun risque de le voir s’envoler.</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A18" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="5">
-        <v>0.75</v>
+      <c r="B18" s="5"/>
+      <c r="C18">
+        <v>13</v>
       </c>
       <c r="E18" s="9">
         <f>F18 / 13</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F18" s="10">
         <f>IF(AND(NOT(ISBLANK(B18)),NOT(ISBLANK(C18))), NA(), IF(NOT(ISBLANK(B18)),B18 * 13,IF(NOT(ISBLANK(C18)),C18, NA())))</f>
-        <v>9.75</v>
+        <v>13</v>
       </c>
       <c r="G18" s="10" t="str">
         <f>IF(cthm_C2_I3_points / 13 &gt;= 0.9,"Excellent", IF(cthm_C2_I3_points / 13 &gt;= 0.8,"Très bien", IF(cthm_C2_I3_points / 13 &gt;= 0.7,"Bien", IF(cthm_C2_I3_points / 13 &gt;= 0.6,"Passable", IF(cthm_C2_I3_points / 13 &gt;= 0,"Insuffisant", "")))))</f>
-        <v>Bien</v>
+        <v>Excellent</v>
       </c>
       <c r="H18" s="10" t="str">
         <f>IF(cthm_C2_I3_points / 13 &gt;= 0.9,"Tendue comme un étai prêt à affronter la plus rude tempête.", IF(cthm_C2_I3_points / 13 &gt;= 0.8,"Bonne tension, un petit relâchement sous forte traction.", IF(cthm_C2_I3_points / 13 &gt;= 0.7,"Correcte mais le nœud principal mérite d’être retendu.", IF(cthm_C2_I3_points / 13 &gt;= 0.6,"Tension inégale, la drisse gondole par endroits.", IF(cthm_C2_I3_points / 13 &gt;= 0,"Molle comme une voile en panne, prête à céder au premier souffle.", "")))))</f>
-        <v>Correcte mais le nœud principal mérite d’être retendu.</v>
+        <v>Tendue comme un étai prêt à affronter la plus rude tempête.</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">

</xml_diff>